<commit_message>
Journal d'activité mis à jour
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal d'activité.xlsx
+++ b/Journal d'activité/Journal d'activité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal Hebdo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4717FC48-FCF4-4567-9C43-A3E54B16A182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA1803B-1DE2-45F8-866E-922833F855E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -61,6 +61,9 @@
   <si>
     <t>Réalisation du schéma réseau de la connexion WiFi de la Raspberry PI 3, de l'ordinateur hébergant le serveur Web et le serveur BDD ainsi que la Box internet de la société</t>
   </si>
+  <si>
+    <t>Travail sur un tutoriel de la configuratrion IP fixe pour la société 13ème Porte</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +72,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,15 +161,6 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,98 +346,98 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -766,74 +760,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="34"/>
+    <col min="1" max="1" width="11.42578125" style="22"/>
     <col min="2" max="2" width="49.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="15"/>
+    <col min="4" max="4" width="11.42578125" style="9"/>
     <col min="5" max="5" width="44.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="15"/>
+    <col min="7" max="7" width="11.42578125" style="9"/>
     <col min="8" max="8" width="42.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="18"/>
+    <col min="10" max="10" width="11.42578125" style="10"/>
     <col min="11" max="11" width="34.42578125" style="2" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="10" customWidth="1"/>
     <col min="14" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="16"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="20">
         <v>43844</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="17"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
+      <c r="A3" s="20">
         <v>43845</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="H3" s="3"/>
@@ -842,19 +836,19 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
+      <c r="A4" s="20">
         <v>43846</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="A5" s="20">
         <v>43847</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
       <c r="H5" s="3"/>
@@ -863,35 +857,35 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="A6" s="20">
         <v>43848</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
+      <c r="A7" s="20">
         <v>43849</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
+      <c r="A8" s="20">
         <v>43850</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="A9" s="20">
         <v>43851</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="H9" s="3"/>
@@ -900,11 +894,11 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
+      <c r="A10" s="20">
         <v>43852</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="H10" s="3"/>
@@ -913,51 +907,51 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
+      <c r="A11" s="20">
         <v>43853</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="32">
+      <c r="A12" s="20">
         <v>43854</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+      <c r="A13" s="20">
         <v>43855</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
+      <c r="A14" s="20">
         <v>43856</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+      <c r="A15" s="20">
         <v>43857</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="A16" s="20">
         <v>43858</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="H16" s="3"/>
@@ -966,11 +960,11 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
+      <c r="A17" s="20">
         <v>43859</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="H17" s="3"/>
@@ -979,54 +973,54 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
+      <c r="A18" s="20">
         <v>43860</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
+      <c r="A19" s="20">
         <v>43861</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
+      <c r="A20" s="20">
         <v>43862</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="32">
+      <c r="A21" s="20">
         <v>43863</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="32">
+      <c r="A22" s="20">
         <v>43864</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="32">
+      <c r="A23" s="20">
         <v>43865</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="9"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="H23" s="3"/>
@@ -1035,11 +1029,11 @@
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="32">
+      <c r="A24" s="20">
         <v>43866</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="H24" s="3"/>
@@ -1048,19 +1042,19 @@
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
+      <c r="A25" s="20">
         <v>43867</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="32">
+      <c r="A26" s="20">
         <v>43868</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
       <c r="H26" s="3"/>
@@ -1069,35 +1063,35 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="32">
+      <c r="A27" s="20">
         <v>43869</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="32">
+      <c r="A28" s="20">
         <v>43870</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="32">
+      <c r="A29" s="20">
         <v>43871</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="32">
+      <c r="A30" s="20">
         <v>43872</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="H30" s="3"/>
@@ -1106,11 +1100,11 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="32">
+      <c r="A31" s="20">
         <v>43873</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="H31" s="3"/>
@@ -1119,19 +1113,19 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="32">
+      <c r="A32" s="20">
         <v>43874</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="32">
+      <c r="A33" s="20">
         <v>43875</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="H33" s="3"/>
@@ -1140,143 +1134,143 @@
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="32">
+      <c r="A34" s="20">
         <v>43876</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="32">
+      <c r="A35" s="20">
         <v>43877</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="32">
+      <c r="A36" s="20">
         <v>43878</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="32">
+      <c r="A37" s="20">
         <v>43879</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="32">
+      <c r="A38" s="20">
         <v>43880</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="32">
+      <c r="A39" s="20">
         <v>43881</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="32">
+      <c r="A40" s="20">
         <v>43882</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="9"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="32">
+      <c r="A41" s="20">
         <v>43883</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="9"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="35"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="32">
+      <c r="A42" s="20">
         <v>43884</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="9"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="32">
+      <c r="A43" s="20">
         <v>43885</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="9"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="32">
+      <c r="A44" s="20">
         <v>43886</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="9"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="35"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="32">
+      <c r="A45" s="20">
         <v>43887</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="9"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
       <c r="F45" s="4"/>
       <c r="H45" s="5"/>
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="32">
+      <c r="A46" s="20">
         <v>43888</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="32">
+      <c r="A47" s="20">
         <v>43889</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="35"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="32">
+      <c r="A48" s="20">
         <v>43890</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="9"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="35"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="32">
+      <c r="A49" s="20">
         <v>43891</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="9"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="32">
+      <c r="A50" s="20">
         <v>43892</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="9"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="32">
+      <c r="A51" s="20">
         <v>43893</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="9"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="35"/>
       <c r="F51" s="4"/>
       <c r="H51" s="5"/>
       <c r="I51" s="1"/>
@@ -1284,11 +1278,11 @@
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="32">
+      <c r="A52" s="20">
         <v>43894</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="9"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="35"/>
       <c r="F52" s="4"/>
       <c r="H52" s="5"/>
       <c r="I52" s="1"/>
@@ -1296,18 +1290,18 @@
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="32">
+      <c r="A53" s="20">
         <v>43895</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="9"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="32">
+      <c r="A54" s="20">
         <v>43896</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="9"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="35"/>
       <c r="F54" s="4"/>
       <c r="H54" s="5"/>
       <c r="I54" s="1"/>
@@ -1315,32 +1309,32 @@
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="32">
+      <c r="A55" s="20">
         <v>43897</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="9"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="32">
+      <c r="A56" s="20">
         <v>43898</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="9"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="32">
+      <c r="A57" s="20">
         <v>43899</v>
       </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="9"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="32">
+      <c r="A58" s="20">
         <v>43900</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="9"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
       <c r="F58" s="4"/>
       <c r="H58" s="5"/>
       <c r="I58" s="1"/>
@@ -1348,11 +1342,11 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="32">
+      <c r="A59" s="20">
         <v>43901</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="9"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="35"/>
       <c r="F59" s="4"/>
       <c r="H59" s="5"/>
       <c r="I59" s="1"/>
@@ -1360,18 +1354,18 @@
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="32">
+      <c r="A60" s="20">
         <v>43902</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="9"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="35"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="32">
+      <c r="A61" s="20">
         <v>43903</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="9"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
       <c r="F61" s="4"/>
       <c r="H61" s="5"/>
       <c r="I61" s="1"/>
@@ -1379,25 +1373,25 @@
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="32">
+      <c r="A62" s="20">
         <v>43904</v>
       </c>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="32">
+      <c r="A63" s="20">
         <v>43905</v>
       </c>
       <c r="B63" s="3"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="32">
+      <c r="A64" s="20">
         <v>43906</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="36">
+      <c r="C64" s="23">
         <v>2</v>
       </c>
       <c r="F64" s="4"/>
@@ -1407,13 +1401,13 @@
       <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="32">
+      <c r="A65" s="20">
         <v>43907</v>
       </c>
-      <c r="B65" s="37" t="s">
+      <c r="B65" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="38">
+      <c r="C65" s="36">
         <v>10</v>
       </c>
       <c r="F65" s="4"/>
@@ -1423,11 +1417,11 @@
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="32">
+      <c r="A66" s="20">
         <v>43908</v>
       </c>
-      <c r="B66" s="37"/>
-      <c r="C66" s="38"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="36"/>
       <c r="F66" s="4"/>
       <c r="H66" s="5"/>
       <c r="I66" s="1"/>
@@ -1435,11 +1429,11 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="32">
+      <c r="A67" s="20">
         <v>43909</v>
       </c>
-      <c r="B67" s="37"/>
-      <c r="C67" s="38"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="36"/>
       <c r="F67" s="4"/>
       <c r="H67" s="5"/>
       <c r="I67" s="1"/>
@@ -1447,561 +1441,649 @@
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="32">
+      <c r="A68" s="20">
         <v>43910</v>
       </c>
-      <c r="B68" s="37"/>
-      <c r="C68" s="38"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="36"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="32">
+      <c r="A69" s="20">
         <v>43911</v>
       </c>
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="39">
+      <c r="C69" s="37">
         <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="32">
+      <c r="A70" s="20">
         <v>43912</v>
       </c>
-      <c r="B70" s="37"/>
-      <c r="C70" s="39"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="37"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="32">
+      <c r="A71" s="20">
         <v>43913</v>
       </c>
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="36">
+      <c r="C71" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="32">
+    <row r="72" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="20">
         <v>43914</v>
       </c>
-      <c r="B72" s="3"/>
+      <c r="B72" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="23">
+        <v>2</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="32">
+      <c r="A73" s="20">
         <v>43915</v>
       </c>
-      <c r="B73" s="3"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="23"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="32">
+      <c r="A74" s="20">
         <v>43916</v>
       </c>
-      <c r="B74" s="3"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="23"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="32">
+      <c r="A75" s="20">
         <v>43917</v>
       </c>
-      <c r="B75" s="3"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="23"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="32">
+      <c r="A76" s="20">
         <v>43918</v>
       </c>
-      <c r="B76" s="3"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="23"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="32">
+      <c r="A77" s="20">
         <v>43919</v>
       </c>
-      <c r="B77" s="3"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="23"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="32">
+      <c r="A78" s="20">
         <v>43920</v>
       </c>
-      <c r="B78" s="3"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="23"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="32">
+      <c r="A79" s="20">
         <v>43921</v>
       </c>
-      <c r="B79" s="3"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="23"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="32">
+      <c r="A80" s="20">
         <v>43922</v>
       </c>
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="32">
+      <c r="B80" s="38"/>
+      <c r="C80" s="23"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
         <v>43923</v>
       </c>
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="32">
+      <c r="B81" s="38"/>
+      <c r="C81" s="23"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
         <v>43924</v>
       </c>
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="32">
+      <c r="B82" s="38"/>
+      <c r="C82" s="23"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
         <v>43925</v>
       </c>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="32">
+      <c r="B83" s="38"/>
+      <c r="C83" s="23"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
         <v>43926</v>
       </c>
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="32">
+      <c r="B84" s="38"/>
+      <c r="C84" s="23"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
         <v>43927</v>
       </c>
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="32">
+      <c r="B85" s="38"/>
+      <c r="C85" s="23"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="20">
         <v>43928</v>
       </c>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="32">
+      <c r="B86" s="38"/>
+      <c r="C86" s="23"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="20">
         <v>43929</v>
       </c>
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="32">
+      <c r="B87" s="38"/>
+      <c r="C87" s="23"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="20">
         <v>43930</v>
       </c>
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="32">
+      <c r="B88" s="38"/>
+      <c r="C88" s="23"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="20">
         <v>43931</v>
       </c>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="32">
+      <c r="B89" s="38"/>
+      <c r="C89" s="23"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
         <v>43932</v>
       </c>
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="32">
+      <c r="B90" s="38"/>
+      <c r="C90" s="23"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
         <v>43933</v>
       </c>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="32">
+      <c r="B91" s="38"/>
+      <c r="C91" s="23"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="20">
         <v>43934</v>
       </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="32">
+      <c r="B92" s="38"/>
+      <c r="C92" s="23"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="20">
         <v>43935</v>
       </c>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="32">
+      <c r="B93" s="38"/>
+      <c r="C93" s="23"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="20">
         <v>43936</v>
       </c>
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="32">
+      <c r="B94" s="38"/>
+      <c r="C94" s="23"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="20">
         <v>43937</v>
       </c>
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="32">
+      <c r="B95" s="38"/>
+      <c r="C95" s="23"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="20">
         <v>43938</v>
       </c>
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="32">
+      <c r="B96" s="38"/>
+      <c r="C96" s="23"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
         <v>43939</v>
       </c>
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="32">
+      <c r="B97" s="38"/>
+      <c r="C97" s="23"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
         <v>43940</v>
       </c>
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="32">
+      <c r="B98" s="38"/>
+      <c r="C98" s="23"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="20">
         <v>43941</v>
       </c>
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="32">
+      <c r="B99" s="38"/>
+      <c r="C99" s="23"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
         <v>43942</v>
       </c>
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="32">
+      <c r="B100" s="38"/>
+      <c r="C100" s="23"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="20">
         <v>43943</v>
       </c>
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="32">
+      <c r="B101" s="38"/>
+      <c r="C101" s="23"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="20">
         <v>43944</v>
       </c>
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="32">
+      <c r="B102" s="38"/>
+      <c r="C102" s="23"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="20">
         <v>43945</v>
       </c>
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="32">
+      <c r="B103" s="38"/>
+      <c r="C103" s="23"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="20">
         <v>43946</v>
       </c>
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="32">
+      <c r="B104" s="38"/>
+      <c r="C104" s="23"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="20">
         <v>43947</v>
       </c>
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="32">
+      <c r="B105" s="38"/>
+      <c r="C105" s="23"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="20">
         <v>43948</v>
       </c>
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="32">
+      <c r="B106" s="38"/>
+      <c r="C106" s="23"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="20">
         <v>43949</v>
       </c>
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="32">
+      <c r="B107" s="38"/>
+      <c r="C107" s="23"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="20">
         <v>43950</v>
       </c>
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="32">
+      <c r="B108" s="38"/>
+      <c r="C108" s="23"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="20">
         <v>43951</v>
       </c>
-      <c r="B109" s="3"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="32">
+      <c r="B109" s="38"/>
+      <c r="C109" s="23"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="20">
         <v>43952</v>
       </c>
-      <c r="B110" s="3"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="32">
+      <c r="B110" s="38"/>
+      <c r="C110" s="23"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="20">
         <v>43953</v>
       </c>
-      <c r="B111" s="3"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="32">
+      <c r="B111" s="38"/>
+      <c r="C111" s="23"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
         <v>43954</v>
       </c>
-      <c r="B112" s="3"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="32">
+      <c r="B112" s="38"/>
+      <c r="C112" s="23"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
         <v>43955</v>
       </c>
-      <c r="B113" s="3"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="32">
+      <c r="B113" s="38"/>
+      <c r="C113" s="23"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
         <v>43956</v>
       </c>
-      <c r="B114" s="3"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="32">
+      <c r="B114" s="38"/>
+      <c r="C114" s="23"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
         <v>43957</v>
       </c>
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="32">
+      <c r="B115" s="38"/>
+      <c r="C115" s="23"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="20">
         <v>43958</v>
       </c>
-      <c r="B116" s="3"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="32">
+      <c r="B116" s="38"/>
+      <c r="C116" s="23"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="20">
         <v>43959</v>
       </c>
-      <c r="B117" s="3"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="32">
+      <c r="B117" s="38"/>
+      <c r="C117" s="23"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="20">
         <v>43960</v>
       </c>
-      <c r="B118" s="3"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="32">
+      <c r="B118" s="38"/>
+      <c r="C118" s="23"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="20">
         <v>43961</v>
       </c>
-      <c r="B119" s="3"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="32">
+      <c r="B119" s="38"/>
+      <c r="C119" s="23"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="20">
         <v>43962</v>
       </c>
-      <c r="B120" s="3"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="32">
+      <c r="B120" s="38"/>
+      <c r="C120" s="23"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="20">
         <v>43963</v>
       </c>
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="32">
+      <c r="B121" s="38"/>
+      <c r="C121" s="23"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="20">
         <v>43964</v>
       </c>
-      <c r="B122" s="3"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="32">
+      <c r="B122" s="38"/>
+      <c r="C122" s="23"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="20">
         <v>43965</v>
       </c>
-      <c r="B123" s="3"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="32">
+      <c r="B123" s="38"/>
+      <c r="C123" s="23"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="20">
         <v>43966</v>
       </c>
-      <c r="B124" s="3"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="32">
+      <c r="B124" s="38"/>
+      <c r="C124" s="23"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="20">
         <v>43967</v>
       </c>
-      <c r="B125" s="3"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="32">
+      <c r="B125" s="38"/>
+      <c r="C125" s="23"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="20">
         <v>43968</v>
       </c>
-      <c r="B126" s="3"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="32">
+      <c r="B126" s="38"/>
+      <c r="C126" s="23"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="20">
         <v>43969</v>
       </c>
-      <c r="B127" s="3"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="32">
+      <c r="B127" s="38"/>
+      <c r="C127" s="23"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="20">
         <v>43970</v>
       </c>
-      <c r="B128" s="3"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="32">
+      <c r="B128" s="38"/>
+      <c r="C128" s="23"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="20">
         <v>43971</v>
       </c>
-      <c r="B129" s="3"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="32">
+      <c r="B129" s="38"/>
+      <c r="C129" s="23"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="20">
         <v>43972</v>
       </c>
-      <c r="B130" s="3"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="32">
+      <c r="B130" s="38"/>
+      <c r="C130" s="23"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="20">
         <v>43973</v>
       </c>
-      <c r="B131" s="3"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="32">
+      <c r="B131" s="38"/>
+      <c r="C131" s="23"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="20">
         <v>43974</v>
       </c>
-      <c r="B132" s="3"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="32">
+      <c r="B132" s="38"/>
+      <c r="C132" s="23"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="20">
         <v>43975</v>
       </c>
-      <c r="B133" s="3"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="32">
+      <c r="B133" s="38"/>
+      <c r="C133" s="23"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="20">
         <v>43976</v>
       </c>
-      <c r="B134" s="3"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="32">
+      <c r="B134" s="38"/>
+      <c r="C134" s="23"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="20">
         <v>43977</v>
       </c>
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="32">
+      <c r="B135" s="38"/>
+      <c r="C135" s="23"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="20">
         <v>43978</v>
       </c>
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="32">
+      <c r="B136" s="38"/>
+      <c r="C136" s="23"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="20">
         <v>43979</v>
       </c>
-      <c r="B137" s="3"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="32">
+      <c r="B137" s="38"/>
+      <c r="C137" s="23"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="20">
         <v>43980</v>
       </c>
-      <c r="B138" s="3"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="32">
+      <c r="B138" s="38"/>
+      <c r="C138" s="23"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="20">
         <v>43981</v>
       </c>
-      <c r="B139" s="3"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="32">
+      <c r="B139" s="38"/>
+      <c r="C139" s="23"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="20">
         <v>43982</v>
       </c>
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="32">
+      <c r="B140" s="38"/>
+      <c r="C140" s="23"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="20">
         <v>43983</v>
       </c>
-      <c r="B141" s="3"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="32">
+      <c r="B141" s="38"/>
+      <c r="C141" s="23"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="20">
         <v>43984</v>
       </c>
-      <c r="B142" s="3"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="32">
+      <c r="B142" s="38"/>
+      <c r="C142" s="23"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="20">
         <v>43985</v>
       </c>
-      <c r="B143" s="3"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="32">
+      <c r="B143" s="38"/>
+      <c r="C143" s="23"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="20">
         <v>43986</v>
       </c>
-      <c r="B144" s="3"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="23"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" s="32">
+      <c r="A145" s="20">
         <v>43987</v>
       </c>
-      <c r="B145" s="3"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="23"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" s="32">
+      <c r="A146" s="20">
         <v>43988</v>
       </c>
-      <c r="B146" s="3"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="23"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="32">
+      <c r="A147" s="20">
         <v>43989</v>
       </c>
-      <c r="B147" s="3"/>
+      <c r="B147" s="38"/>
+      <c r="C147" s="23"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" s="32">
+      <c r="A148" s="20">
         <v>43990</v>
       </c>
-      <c r="B148" s="3"/>
+      <c r="B148" s="38"/>
+      <c r="C148" s="23"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" s="32">
+      <c r="A149" s="20">
         <v>43991</v>
       </c>
-      <c r="B149" s="3"/>
+      <c r="B149" s="38"/>
+      <c r="C149" s="23"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="32">
+      <c r="A150" s="20">
         <v>43992</v>
       </c>
-      <c r="B150" s="3"/>
+      <c r="B150" s="38"/>
+      <c r="C150" s="23"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A151" s="32">
+      <c r="A151" s="20">
         <v>43993</v>
       </c>
-      <c r="B151" s="3"/>
+      <c r="B151" s="38"/>
+      <c r="C151" s="23"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A152" s="32">
+      <c r="A152" s="20">
         <v>43994</v>
       </c>
-      <c r="B152" s="3"/>
+      <c r="B152" s="38"/>
+      <c r="C152" s="23"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" s="32">
+      <c r="A153" s="20">
         <v>43995</v>
       </c>
-      <c r="B153" s="3"/>
+      <c r="B153" s="38"/>
+      <c r="C153" s="23"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" s="32">
+      <c r="A154" s="20">
         <v>43996</v>
       </c>
-      <c r="B154" s="3"/>
+      <c r="B154" s="38"/>
+      <c r="C154" s="23"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A155" s="32">
+      <c r="A155" s="20">
         <v>43997</v>
       </c>
-      <c r="B155" s="3"/>
+      <c r="B155" s="38"/>
+      <c r="C155" s="23"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A156" s="33"/>
+      <c r="A156" s="21"/>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A157" s="33"/>
+      <c r="A157" s="21"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A158" s="33"/>
+      <c r="A158" s="21"/>
     </row>
     <row r="159" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="19" t="s">
+      <c r="A159" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C159" s="21">
+      <c r="C159" s="13">
         <f>SUM(C64:C155)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F159" s="6">
         <f>SUM(F2:F155)</f>
@@ -2019,15 +2101,15 @@
     <row r="160" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C61"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificatoin du journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal d'activité.xlsx
+++ b/Journal d'activité/Journal d'activité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA1803B-1DE2-45F8-866E-922833F855E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541D2C5F-8C2F-482B-9524-45AC734BAE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -391,6 +391,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,25 +430,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,42 +792,42 @@
       <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="26"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
-      <c r="J1" s="28"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
-      <c r="M1" s="30"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>43844</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="16"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="27"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="16"/>
       <c r="I2" s="18"/>
-      <c r="J2" s="29"/>
+      <c r="J2" s="33"/>
       <c r="K2" s="16"/>
       <c r="L2" s="18"/>
-      <c r="M2" s="31"/>
+      <c r="M2" s="35"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>43845</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="H3" s="3"/>
@@ -839,16 +839,16 @@
       <c r="A4" s="20">
         <v>43846</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>43847</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
       <c r="H5" s="3"/>
@@ -860,32 +860,32 @@
       <c r="A6" s="20">
         <v>43848</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>43849</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>43850</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>43851</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="H9" s="3"/>
@@ -897,8 +897,8 @@
       <c r="A10" s="20">
         <v>43852</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="H10" s="3"/>
@@ -910,48 +910,48 @@
       <c r="A11" s="20">
         <v>43853</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>43854</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>43855</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>43856</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>43857</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>43858</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="H16" s="3"/>
@@ -963,8 +963,8 @@
       <c r="A17" s="20">
         <v>43859</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="H17" s="3"/>
@@ -976,16 +976,16 @@
       <c r="A18" s="20">
         <v>43860</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>43861</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="I19" s="1"/>
@@ -995,32 +995,32 @@
       <c r="A20" s="20">
         <v>43862</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>43863</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>43864</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>43865</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="H23" s="3"/>
@@ -1032,8 +1032,8 @@
       <c r="A24" s="20">
         <v>43866</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="H24" s="3"/>
@@ -1045,16 +1045,16 @@
       <c r="A25" s="20">
         <v>43867</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>43868</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
       <c r="H26" s="3"/>
@@ -1066,32 +1066,32 @@
       <c r="A27" s="20">
         <v>43869</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>43870</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <v>43871</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>43872</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="H30" s="3"/>
@@ -1103,8 +1103,8 @@
       <c r="A31" s="20">
         <v>43873</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="H31" s="3"/>
@@ -1116,16 +1116,16 @@
       <c r="A32" s="20">
         <v>43874</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="35"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>43875</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="H33" s="3"/>
@@ -1137,95 +1137,95 @@
       <c r="A34" s="20">
         <v>43876</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="35"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>43877</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>43878</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>43879</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <v>43880</v>
       </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>43881</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="35"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>43882</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="39"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>43883</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>43884</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="39"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>43885</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>43886</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="35"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>43887</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="35"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
       <c r="F45" s="4"/>
       <c r="H45" s="5"/>
       <c r="K45" s="5"/>
@@ -1234,43 +1234,43 @@
       <c r="A46" s="20">
         <v>43888</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="35"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="39"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
         <v>43889</v>
       </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="35"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>43890</v>
       </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="35"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="39"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>43891</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="35"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="39"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <v>43892</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>43893</v>
       </c>
-      <c r="B51" s="34"/>
-      <c r="C51" s="35"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="39"/>
       <c r="F51" s="4"/>
       <c r="H51" s="5"/>
       <c r="I51" s="1"/>
@@ -1281,8 +1281,8 @@
       <c r="A52" s="20">
         <v>43894</v>
       </c>
-      <c r="B52" s="34"/>
-      <c r="C52" s="35"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="39"/>
       <c r="F52" s="4"/>
       <c r="H52" s="5"/>
       <c r="I52" s="1"/>
@@ -1293,15 +1293,15 @@
       <c r="A53" s="20">
         <v>43895</v>
       </c>
-      <c r="B53" s="34"/>
-      <c r="C53" s="35"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="39"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>43896</v>
       </c>
-      <c r="B54" s="34"/>
-      <c r="C54" s="35"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="39"/>
       <c r="F54" s="4"/>
       <c r="H54" s="5"/>
       <c r="I54" s="1"/>
@@ -1312,29 +1312,29 @@
       <c r="A55" s="20">
         <v>43897</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="35"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="39"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>43898</v>
       </c>
-      <c r="B56" s="34"/>
-      <c r="C56" s="35"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="39"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>43899</v>
       </c>
-      <c r="B57" s="34"/>
-      <c r="C57" s="35"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="39"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <v>43900</v>
       </c>
-      <c r="B58" s="34"/>
-      <c r="C58" s="35"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
       <c r="F58" s="4"/>
       <c r="H58" s="5"/>
       <c r="I58" s="1"/>
@@ -1345,8 +1345,8 @@
       <c r="A59" s="20">
         <v>43901</v>
       </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="35"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
       <c r="F59" s="4"/>
       <c r="H59" s="5"/>
       <c r="I59" s="1"/>
@@ -1357,15 +1357,15 @@
       <c r="A60" s="20">
         <v>43902</v>
       </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="35"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>43903</v>
       </c>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="39"/>
       <c r="F61" s="4"/>
       <c r="H61" s="5"/>
       <c r="I61" s="1"/>
@@ -1376,19 +1376,21 @@
       <c r="A62" s="20">
         <v>43904</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="39"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>43905</v>
       </c>
-      <c r="B63" s="3"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="39"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
         <v>43906</v>
       </c>
-      <c r="B64" s="38" t="s">
+      <c r="B64" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="23">
@@ -1404,10 +1406,10 @@
       <c r="A65" s="20">
         <v>43907</v>
       </c>
-      <c r="B65" s="39" t="s">
+      <c r="B65" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="36">
+      <c r="C65" s="26">
         <v>10</v>
       </c>
       <c r="F65" s="4"/>
@@ -1420,8 +1422,8 @@
       <c r="A66" s="20">
         <v>43908</v>
       </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="36"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="26"/>
       <c r="F66" s="4"/>
       <c r="H66" s="5"/>
       <c r="I66" s="1"/>
@@ -1432,8 +1434,8 @@
       <c r="A67" s="20">
         <v>43909</v>
       </c>
-      <c r="B67" s="39"/>
-      <c r="C67" s="36"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="26"/>
       <c r="F67" s="4"/>
       <c r="H67" s="5"/>
       <c r="I67" s="1"/>
@@ -1444,17 +1446,17 @@
       <c r="A68" s="20">
         <v>43910</v>
       </c>
-      <c r="B68" s="39"/>
-      <c r="C68" s="36"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="26"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="20">
         <v>43911</v>
       </c>
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="37">
+      <c r="C69" s="27">
         <v>4</v>
       </c>
     </row>
@@ -1462,14 +1464,14 @@
       <c r="A70" s="20">
         <v>43912</v>
       </c>
-      <c r="B70" s="39"/>
-      <c r="C70" s="37"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="27"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
         <v>43913</v>
       </c>
-      <c r="B71" s="38" t="s">
+      <c r="B71" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="23">
@@ -1480,7 +1482,7 @@
       <c r="A72" s="20">
         <v>43914</v>
       </c>
-      <c r="B72" s="38" t="s">
+      <c r="B72" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="23">
@@ -1491,581 +1493,581 @@
       <c r="A73" s="20">
         <v>43915</v>
       </c>
-      <c r="B73" s="38"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="23"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
         <v>43916</v>
       </c>
-      <c r="B74" s="38"/>
+      <c r="B74" s="24"/>
       <c r="C74" s="23"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
         <v>43917</v>
       </c>
-      <c r="B75" s="38"/>
+      <c r="B75" s="24"/>
       <c r="C75" s="23"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
         <v>43918</v>
       </c>
-      <c r="B76" s="38"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="23"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
         <v>43919</v>
       </c>
-      <c r="B77" s="38"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="23"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
         <v>43920</v>
       </c>
-      <c r="B78" s="38"/>
+      <c r="B78" s="24"/>
       <c r="C78" s="23"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
         <v>43921</v>
       </c>
-      <c r="B79" s="38"/>
+      <c r="B79" s="24"/>
       <c r="C79" s="23"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>43922</v>
       </c>
-      <c r="B80" s="38"/>
+      <c r="B80" s="24"/>
       <c r="C80" s="23"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
         <v>43923</v>
       </c>
-      <c r="B81" s="38"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="23"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
         <v>43924</v>
       </c>
-      <c r="B82" s="38"/>
+      <c r="B82" s="24"/>
       <c r="C82" s="23"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
         <v>43925</v>
       </c>
-      <c r="B83" s="38"/>
+      <c r="B83" s="24"/>
       <c r="C83" s="23"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
         <v>43926</v>
       </c>
-      <c r="B84" s="38"/>
+      <c r="B84" s="24"/>
       <c r="C84" s="23"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
         <v>43927</v>
       </c>
-      <c r="B85" s="38"/>
+      <c r="B85" s="24"/>
       <c r="C85" s="23"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
         <v>43928</v>
       </c>
-      <c r="B86" s="38"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="23"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="20">
         <v>43929</v>
       </c>
-      <c r="B87" s="38"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="23"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="20">
         <v>43930</v>
       </c>
-      <c r="B88" s="38"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="23"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="20">
         <v>43931</v>
       </c>
-      <c r="B89" s="38"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="23"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="20">
         <v>43932</v>
       </c>
-      <c r="B90" s="38"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="23"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="20">
         <v>43933</v>
       </c>
-      <c r="B91" s="38"/>
+      <c r="B91" s="24"/>
       <c r="C91" s="23"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="20">
         <v>43934</v>
       </c>
-      <c r="B92" s="38"/>
+      <c r="B92" s="24"/>
       <c r="C92" s="23"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="20">
         <v>43935</v>
       </c>
-      <c r="B93" s="38"/>
+      <c r="B93" s="24"/>
       <c r="C93" s="23"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="20">
         <v>43936</v>
       </c>
-      <c r="B94" s="38"/>
+      <c r="B94" s="24"/>
       <c r="C94" s="23"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="20">
         <v>43937</v>
       </c>
-      <c r="B95" s="38"/>
+      <c r="B95" s="24"/>
       <c r="C95" s="23"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="20">
         <v>43938</v>
       </c>
-      <c r="B96" s="38"/>
+      <c r="B96" s="24"/>
       <c r="C96" s="23"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="20">
         <v>43939</v>
       </c>
-      <c r="B97" s="38"/>
+      <c r="B97" s="24"/>
       <c r="C97" s="23"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="20">
         <v>43940</v>
       </c>
-      <c r="B98" s="38"/>
+      <c r="B98" s="24"/>
       <c r="C98" s="23"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="20">
         <v>43941</v>
       </c>
-      <c r="B99" s="38"/>
+      <c r="B99" s="24"/>
       <c r="C99" s="23"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
         <v>43942</v>
       </c>
-      <c r="B100" s="38"/>
+      <c r="B100" s="24"/>
       <c r="C100" s="23"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
         <v>43943</v>
       </c>
-      <c r="B101" s="38"/>
+      <c r="B101" s="24"/>
       <c r="C101" s="23"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="20">
         <v>43944</v>
       </c>
-      <c r="B102" s="38"/>
+      <c r="B102" s="24"/>
       <c r="C102" s="23"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="20">
         <v>43945</v>
       </c>
-      <c r="B103" s="38"/>
+      <c r="B103" s="24"/>
       <c r="C103" s="23"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="20">
         <v>43946</v>
       </c>
-      <c r="B104" s="38"/>
+      <c r="B104" s="24"/>
       <c r="C104" s="23"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="20">
         <v>43947</v>
       </c>
-      <c r="B105" s="38"/>
+      <c r="B105" s="24"/>
       <c r="C105" s="23"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="20">
         <v>43948</v>
       </c>
-      <c r="B106" s="38"/>
+      <c r="B106" s="24"/>
       <c r="C106" s="23"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="20">
         <v>43949</v>
       </c>
-      <c r="B107" s="38"/>
+      <c r="B107" s="24"/>
       <c r="C107" s="23"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="20">
         <v>43950</v>
       </c>
-      <c r="B108" s="38"/>
+      <c r="B108" s="24"/>
       <c r="C108" s="23"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="20">
         <v>43951</v>
       </c>
-      <c r="B109" s="38"/>
+      <c r="B109" s="24"/>
       <c r="C109" s="23"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="20">
         <v>43952</v>
       </c>
-      <c r="B110" s="38"/>
+      <c r="B110" s="24"/>
       <c r="C110" s="23"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="20">
         <v>43953</v>
       </c>
-      <c r="B111" s="38"/>
+      <c r="B111" s="24"/>
       <c r="C111" s="23"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="20">
         <v>43954</v>
       </c>
-      <c r="B112" s="38"/>
+      <c r="B112" s="24"/>
       <c r="C112" s="23"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="20">
         <v>43955</v>
       </c>
-      <c r="B113" s="38"/>
+      <c r="B113" s="24"/>
       <c r="C113" s="23"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="20">
         <v>43956</v>
       </c>
-      <c r="B114" s="38"/>
+      <c r="B114" s="24"/>
       <c r="C114" s="23"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="20">
         <v>43957</v>
       </c>
-      <c r="B115" s="38"/>
+      <c r="B115" s="24"/>
       <c r="C115" s="23"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="20">
         <v>43958</v>
       </c>
-      <c r="B116" s="38"/>
+      <c r="B116" s="24"/>
       <c r="C116" s="23"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="20">
         <v>43959</v>
       </c>
-      <c r="B117" s="38"/>
+      <c r="B117" s="24"/>
       <c r="C117" s="23"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="20">
         <v>43960</v>
       </c>
-      <c r="B118" s="38"/>
+      <c r="B118" s="24"/>
       <c r="C118" s="23"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="20">
         <v>43961</v>
       </c>
-      <c r="B119" s="38"/>
+      <c r="B119" s="24"/>
       <c r="C119" s="23"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="20">
         <v>43962</v>
       </c>
-      <c r="B120" s="38"/>
+      <c r="B120" s="24"/>
       <c r="C120" s="23"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="20">
         <v>43963</v>
       </c>
-      <c r="B121" s="38"/>
+      <c r="B121" s="24"/>
       <c r="C121" s="23"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="20">
         <v>43964</v>
       </c>
-      <c r="B122" s="38"/>
+      <c r="B122" s="24"/>
       <c r="C122" s="23"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="20">
         <v>43965</v>
       </c>
-      <c r="B123" s="38"/>
+      <c r="B123" s="24"/>
       <c r="C123" s="23"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="20">
         <v>43966</v>
       </c>
-      <c r="B124" s="38"/>
+      <c r="B124" s="24"/>
       <c r="C124" s="23"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="20">
         <v>43967</v>
       </c>
-      <c r="B125" s="38"/>
+      <c r="B125" s="24"/>
       <c r="C125" s="23"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="20">
         <v>43968</v>
       </c>
-      <c r="B126" s="38"/>
+      <c r="B126" s="24"/>
       <c r="C126" s="23"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="20">
         <v>43969</v>
       </c>
-      <c r="B127" s="38"/>
+      <c r="B127" s="24"/>
       <c r="C127" s="23"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="20">
         <v>43970</v>
       </c>
-      <c r="B128" s="38"/>
+      <c r="B128" s="24"/>
       <c r="C128" s="23"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="20">
         <v>43971</v>
       </c>
-      <c r="B129" s="38"/>
+      <c r="B129" s="24"/>
       <c r="C129" s="23"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="20">
         <v>43972</v>
       </c>
-      <c r="B130" s="38"/>
+      <c r="B130" s="24"/>
       <c r="C130" s="23"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="20">
         <v>43973</v>
       </c>
-      <c r="B131" s="38"/>
+      <c r="B131" s="24"/>
       <c r="C131" s="23"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="20">
         <v>43974</v>
       </c>
-      <c r="B132" s="38"/>
+      <c r="B132" s="24"/>
       <c r="C132" s="23"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="20">
         <v>43975</v>
       </c>
-      <c r="B133" s="38"/>
+      <c r="B133" s="24"/>
       <c r="C133" s="23"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="20">
         <v>43976</v>
       </c>
-      <c r="B134" s="38"/>
+      <c r="B134" s="24"/>
       <c r="C134" s="23"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="20">
         <v>43977</v>
       </c>
-      <c r="B135" s="38"/>
+      <c r="B135" s="24"/>
       <c r="C135" s="23"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="20">
         <v>43978</v>
       </c>
-      <c r="B136" s="38"/>
+      <c r="B136" s="24"/>
       <c r="C136" s="23"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="20">
         <v>43979</v>
       </c>
-      <c r="B137" s="38"/>
+      <c r="B137" s="24"/>
       <c r="C137" s="23"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="20">
         <v>43980</v>
       </c>
-      <c r="B138" s="38"/>
+      <c r="B138" s="24"/>
       <c r="C138" s="23"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="20">
         <v>43981</v>
       </c>
-      <c r="B139" s="38"/>
+      <c r="B139" s="24"/>
       <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="20">
         <v>43982</v>
       </c>
-      <c r="B140" s="38"/>
+      <c r="B140" s="24"/>
       <c r="C140" s="23"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="20">
         <v>43983</v>
       </c>
-      <c r="B141" s="38"/>
+      <c r="B141" s="24"/>
       <c r="C141" s="23"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="20">
         <v>43984</v>
       </c>
-      <c r="B142" s="38"/>
+      <c r="B142" s="24"/>
       <c r="C142" s="23"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="20">
         <v>43985</v>
       </c>
-      <c r="B143" s="38"/>
+      <c r="B143" s="24"/>
       <c r="C143" s="23"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="20">
         <v>43986</v>
       </c>
-      <c r="B144" s="38"/>
+      <c r="B144" s="24"/>
       <c r="C144" s="23"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="20">
         <v>43987</v>
       </c>
-      <c r="B145" s="38"/>
+      <c r="B145" s="24"/>
       <c r="C145" s="23"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="20">
         <v>43988</v>
       </c>
-      <c r="B146" s="38"/>
+      <c r="B146" s="24"/>
       <c r="C146" s="23"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="20">
         <v>43989</v>
       </c>
-      <c r="B147" s="38"/>
+      <c r="B147" s="24"/>
       <c r="C147" s="23"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="20">
         <v>43990</v>
       </c>
-      <c r="B148" s="38"/>
+      <c r="B148" s="24"/>
       <c r="C148" s="23"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="20">
         <v>43991</v>
       </c>
-      <c r="B149" s="38"/>
+      <c r="B149" s="24"/>
       <c r="C149" s="23"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="20">
         <v>43992</v>
       </c>
-      <c r="B150" s="38"/>
+      <c r="B150" s="24"/>
       <c r="C150" s="23"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="20">
         <v>43993</v>
       </c>
-      <c r="B151" s="38"/>
+      <c r="B151" s="24"/>
       <c r="C151" s="23"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="20">
         <v>43994</v>
       </c>
-      <c r="B152" s="38"/>
+      <c r="B152" s="24"/>
       <c r="C152" s="23"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="20">
         <v>43995</v>
       </c>
-      <c r="B153" s="38"/>
+      <c r="B153" s="24"/>
       <c r="C153" s="23"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="20">
         <v>43996</v>
       </c>
-      <c r="B154" s="38"/>
+      <c r="B154" s="24"/>
       <c r="C154" s="23"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="20">
         <v>43997</v>
       </c>
-      <c r="B155" s="38"/>
+      <c r="B155" s="24"/>
       <c r="C155" s="23"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
@@ -2101,15 +2103,15 @@
     <row r="160" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B2:C63"/>
     <mergeCell ref="B65:B68"/>
     <mergeCell ref="C65:C68"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="B2:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Journal d'activité à jour
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal d'activité.xlsx
+++ b/Journal d'activité/Journal d'activité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totok\Documents\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592CCE81-B641-46FC-A060-52A37476D8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C5FA4E-9686-4484-A583-CCB9DEE2FDA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Choix de logiciel de programmation = Uniquement sur arduino/ Commencer a programmer et à cabler le matériel.</t>
+  </si>
+  <si>
+    <t>Rédaction de ma partie du cahier de recette</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -361,9 +364,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,12 +417,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,42 +470,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -792,919 +792,919 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72:F73"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="20"/>
+    <col min="1" max="1" width="11.42578125" style="19"/>
     <col min="2" max="2" width="49.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="8"/>
+    <col min="4" max="4" width="11.42578125" style="7"/>
     <col min="5" max="5" width="44.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="8"/>
+    <col min="7" max="7" width="11.42578125" style="7"/>
     <col min="8" max="8" width="42.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="9"/>
+    <col min="10" max="10" width="11.42578125" style="8"/>
     <col min="11" max="11" width="34.42578125" style="2" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="8" customWidth="1"/>
     <col min="14" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="30"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="26"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="31"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="32" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="29"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="18">
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="17">
         <v>43845</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="18">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="17">
         <v>43846</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="18">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="17">
         <v>43847</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="18">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="17">
         <v>43848</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="18">
+      <c r="B8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="17">
         <v>43849</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="18">
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="17">
         <v>43850</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="18">
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="17">
         <v>43851</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="18">
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="17">
         <v>43852</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="18">
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="17">
         <v>43853</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="18">
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="17">
         <v>43854</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="18">
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="17">
         <v>43855</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="35"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="18">
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="17">
         <v>43856</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+      <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="18">
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="17">
         <v>43857</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+      <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="18">
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="17">
         <v>43858</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="18">
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="17">
         <v>43859</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="18">
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="17">
         <v>43860</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+      <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="18">
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="17">
         <v>43861</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="18">
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="17">
         <v>43862</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+      <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="18">
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="17">
         <v>43863</v>
       </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
+      <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="18">
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="17">
         <v>43864</v>
       </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18">
+      <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="18">
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="17">
         <v>43865</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
+      <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="18">
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="17">
         <v>43866</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="18">
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="17">
         <v>43867</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="18">
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="17">
         <v>43868</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18">
+      <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="18">
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="17">
         <v>43869</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18">
+      <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="18">
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="17">
         <v>43870</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18">
+      <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="18">
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="17">
         <v>43871</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="31"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18">
+      <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="18">
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="17">
         <v>43872</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18">
+      <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="18">
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="17">
         <v>43873</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="31"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18">
+      <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="18">
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="17">
         <v>43874</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18">
+      <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="18">
+      <c r="B34" s="30"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="17">
         <v>43875</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="35"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
+      <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="18">
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="17">
         <v>43876</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18">
+      <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="18">
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="17">
         <v>43877</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="35"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18">
+      <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="18">
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="17">
         <v>43878</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18">
+      <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="18">
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="17">
         <v>43879</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="35"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18">
+      <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="18">
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="17">
         <v>43880</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="35"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18">
+      <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="18">
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="17">
         <v>43881</v>
       </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="35"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="31"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18">
+      <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="18">
+      <c r="B41" s="30"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="17">
         <v>43882</v>
       </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="35"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="31"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
+      <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="18">
+      <c r="B42" s="30"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="17">
         <v>43883</v>
       </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="35"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="31"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18">
+      <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="18">
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="17">
         <v>43884</v>
       </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="35"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="31"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18">
+      <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="18">
+      <c r="B44" s="30"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="17">
         <v>43885</v>
       </c>
-      <c r="E44" s="34"/>
-      <c r="F44" s="35"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="31"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
+      <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="18">
+      <c r="B45" s="30"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="17">
         <v>43886</v>
       </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="35"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="31"/>
       <c r="H45" s="4"/>
       <c r="K45" s="4"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18">
+      <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="18">
+      <c r="B46" s="30"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="17">
         <v>43887</v>
       </c>
-      <c r="E46" s="34"/>
-      <c r="F46" s="35"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="31"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18">
+      <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="18">
+      <c r="B47" s="30"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="17">
         <v>43888</v>
       </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="35"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="31"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18">
+      <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="18">
+      <c r="B48" s="30"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="17">
         <v>43889</v>
       </c>
-      <c r="E48" s="34"/>
-      <c r="F48" s="35"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="31"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18">
+      <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="18">
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="17">
         <v>43890</v>
       </c>
-      <c r="E49" s="34"/>
-      <c r="F49" s="35"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="31"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+      <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="18">
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="17">
         <v>43891</v>
       </c>
-      <c r="E50" s="34"/>
-      <c r="F50" s="35"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="31"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18">
+      <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="34"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="18">
+      <c r="B51" s="30"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="17">
         <v>43892</v>
       </c>
-      <c r="E51" s="34"/>
-      <c r="F51" s="35"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="31"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
       <c r="K51" s="4"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
+      <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="34"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="18">
+      <c r="B52" s="30"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="17">
         <v>43893</v>
       </c>
-      <c r="E52" s="34"/>
-      <c r="F52" s="35"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="31"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
       <c r="K52" s="4"/>
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18">
+      <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="34"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="18">
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="17">
         <v>43894</v>
       </c>
-      <c r="E53" s="34"/>
-      <c r="F53" s="35"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="31"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18">
+      <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="34"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="18">
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="17">
         <v>43895</v>
       </c>
-      <c r="E54" s="34"/>
-      <c r="F54" s="35"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
       <c r="K54" s="4"/>
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18">
+      <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="18">
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="17">
         <v>43896</v>
       </c>
-      <c r="E55" s="34"/>
-      <c r="F55" s="35"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="31"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18">
+      <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="34"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="18">
+      <c r="B56" s="30"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="17">
         <v>43897</v>
       </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="35"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="31"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18">
+      <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="34"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="18">
+      <c r="B57" s="30"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="17">
         <v>43898</v>
       </c>
-      <c r="E57" s="34"/>
-      <c r="F57" s="35"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="31"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18">
+      <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="34"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="18">
+      <c r="B58" s="30"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="17">
         <v>43899</v>
       </c>
-      <c r="E58" s="34"/>
-      <c r="F58" s="35"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="31"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
       <c r="K58" s="4"/>
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18">
+      <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="18">
+      <c r="B59" s="30"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="17">
         <v>43900</v>
       </c>
-      <c r="E59" s="34"/>
-      <c r="F59" s="35"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="31"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="K59" s="4"/>
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18">
+      <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="18">
+      <c r="B60" s="30"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="17">
         <v>43901</v>
       </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="35"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="31"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18">
+      <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="18">
+      <c r="B61" s="30"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="17">
         <v>43902</v>
       </c>
-      <c r="E61" s="34"/>
-      <c r="F61" s="35"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="31"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="K61" s="4"/>
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18">
+      <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="34"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="18">
+      <c r="B62" s="30"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="17">
         <v>43903</v>
       </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="35"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="31"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18">
+      <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="34"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="18">
+      <c r="B63" s="30"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="17">
         <v>43904</v>
       </c>
-      <c r="E63" s="34"/>
-      <c r="F63" s="35"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="31"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18">
+      <c r="A64" s="17">
         <v>43906</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="21">
+      <c r="C64" s="20">
         <v>2</v>
       </c>
-      <c r="D64" s="18">
+      <c r="D64" s="17">
         <v>43905</v>
       </c>
-      <c r="E64" s="34"/>
-      <c r="F64" s="35"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="31"/>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
       <c r="K64" s="4"/>
       <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="18">
+      <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="36">
+      <c r="C65" s="33">
         <v>10</v>
       </c>
-      <c r="D65" s="18">
+      <c r="D65" s="17">
         <v>43906</v>
       </c>
-      <c r="E65" s="22" t="s">
+      <c r="E65" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="23">
+      <c r="F65" s="22">
         <v>2</v>
       </c>
       <c r="H65" s="4"/>
@@ -1713,18 +1713,18 @@
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18">
+      <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="18">
+      <c r="B66" s="32"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="17">
         <v>43907</v>
       </c>
-      <c r="E66" s="24" t="s">
+      <c r="E66" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="36">
+      <c r="F66" s="33">
         <v>13</v>
       </c>
       <c r="H66" s="4"/>
@@ -1733,973 +1733,977 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="18">
+      <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="24"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="18">
+      <c r="B67" s="32"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="17">
         <v>43908</v>
       </c>
-      <c r="E67" s="24"/>
-      <c r="F67" s="36"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="33"/>
       <c r="H67" s="4"/>
       <c r="I67" s="1"/>
       <c r="K67" s="4"/>
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="18">
+      <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="18">
+      <c r="B68" s="32"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="17">
         <v>43909</v>
       </c>
-      <c r="E68" s="24"/>
-      <c r="F68" s="36"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="33"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="18">
+      <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B69" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="25">
+      <c r="C69" s="34">
         <v>4</v>
       </c>
-      <c r="D69" s="18">
+      <c r="D69" s="17">
         <v>43910</v>
       </c>
-      <c r="E69" s="24"/>
-      <c r="F69" s="36"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="33"/>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18">
+      <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="18">
+      <c r="B70" s="32"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="17">
         <v>43911</v>
       </c>
-      <c r="E70" s="24" t="s">
+      <c r="E70" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="41">
+      <c r="F70" s="25">
         <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="18">
+      <c r="A71" s="17">
         <v>43913</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="21">
+      <c r="C71" s="20">
         <v>2</v>
       </c>
-      <c r="D71" s="18">
+      <c r="D71" s="17">
         <v>43912</v>
       </c>
-      <c r="E71" s="24"/>
-      <c r="F71" s="41"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="25"/>
     </row>
     <row r="72" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="18">
+      <c r="A72" s="17">
         <v>43914</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="21">
+      <c r="C72" s="20">
         <v>3</v>
       </c>
-      <c r="D72" s="18">
+      <c r="D72" s="17">
         <v>43913</v>
       </c>
-      <c r="E72" s="40" t="s">
+      <c r="E72" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F72" s="41">
+      <c r="F72" s="25">
         <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="18">
+      <c r="A73" s="17">
         <v>43915</v>
       </c>
-      <c r="B73" s="22"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="18">
+      <c r="B73" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="20">
+        <v>2</v>
+      </c>
+      <c r="D73" s="17">
         <v>43914</v>
       </c>
-      <c r="E73" s="40"/>
-      <c r="F73" s="41"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="25"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="18">
+      <c r="A74" s="17">
         <v>43916</v>
       </c>
-      <c r="B74" s="22"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="18">
+      <c r="B74" s="21"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="17">
         <v>43915</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="18">
+      <c r="A75" s="17">
         <v>43917</v>
       </c>
-      <c r="B75" s="22"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="18">
+      <c r="B75" s="21"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="17">
         <v>43916</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="18">
+      <c r="A76" s="17">
         <v>43918</v>
       </c>
-      <c r="B76" s="22"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="18">
+      <c r="B76" s="21"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="17">
         <v>43917</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="18">
+      <c r="A77" s="17">
         <v>43919</v>
       </c>
-      <c r="B77" s="22"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="18">
+      <c r="B77" s="21"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="17">
         <v>43918</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="18">
+      <c r="A78" s="17">
         <v>43920</v>
       </c>
-      <c r="B78" s="22"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="18">
+      <c r="B78" s="21"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="17">
         <v>43919</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="18">
+      <c r="A79" s="17">
         <v>43921</v>
       </c>
-      <c r="B79" s="22"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="18">
+      <c r="B79" s="21"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="17">
         <v>43920</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="18">
+      <c r="A80" s="17">
         <v>43922</v>
       </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="18">
+      <c r="B80" s="21"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="17">
         <v>43921</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="18">
+      <c r="A81" s="17">
         <v>43923</v>
       </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="18">
+      <c r="B81" s="21"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="17">
         <v>43922</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="18">
+      <c r="A82" s="17">
         <v>43924</v>
       </c>
-      <c r="B82" s="22"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="18">
+      <c r="B82" s="21"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="17">
         <v>43923</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="18">
+      <c r="A83" s="17">
         <v>43925</v>
       </c>
-      <c r="B83" s="22"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="18">
+      <c r="B83" s="21"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="17">
         <v>43924</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="18">
+      <c r="A84" s="17">
         <v>43926</v>
       </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="18">
+      <c r="B84" s="21"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="17">
         <v>43925</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="18">
+      <c r="A85" s="17">
         <v>43927</v>
       </c>
-      <c r="B85" s="22"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="18">
+      <c r="B85" s="21"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="17">
         <v>43926</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="18">
+      <c r="A86" s="17">
         <v>43928</v>
       </c>
-      <c r="B86" s="22"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="18">
+      <c r="B86" s="21"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="17">
         <v>43927</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="18">
+      <c r="A87" s="17">
         <v>43929</v>
       </c>
-      <c r="B87" s="22"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="18">
+      <c r="B87" s="21"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="17">
         <v>43928</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="18">
+      <c r="A88" s="17">
         <v>43930</v>
       </c>
-      <c r="B88" s="22"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="18">
+      <c r="B88" s="21"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="17">
         <v>43929</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="18">
+      <c r="A89" s="17">
         <v>43931</v>
       </c>
-      <c r="B89" s="22"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="18">
+      <c r="B89" s="21"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="17">
         <v>43930</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="18">
+      <c r="A90" s="17">
         <v>43932</v>
       </c>
-      <c r="B90" s="22"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="18">
+      <c r="B90" s="21"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="17">
         <v>43931</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="18">
+      <c r="A91" s="17">
         <v>43933</v>
       </c>
-      <c r="B91" s="22"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="18">
+      <c r="B91" s="21"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="17">
         <v>43932</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="18">
+      <c r="A92" s="17">
         <v>43934</v>
       </c>
-      <c r="B92" s="22"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="18">
+      <c r="B92" s="21"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="17">
         <v>43933</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="18">
+      <c r="A93" s="17">
         <v>43935</v>
       </c>
-      <c r="B93" s="22"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="18">
+      <c r="B93" s="21"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="17">
         <v>43934</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="18">
+      <c r="A94" s="17">
         <v>43936</v>
       </c>
-      <c r="B94" s="22"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="18">
+      <c r="B94" s="21"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="17">
         <v>43935</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="18">
+      <c r="A95" s="17">
         <v>43937</v>
       </c>
-      <c r="B95" s="22"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="18">
+      <c r="B95" s="21"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="17">
         <v>43936</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="18">
+      <c r="A96" s="17">
         <v>43938</v>
       </c>
-      <c r="B96" s="22"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="18">
+      <c r="B96" s="21"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="17">
         <v>43937</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="18">
+      <c r="A97" s="17">
         <v>43939</v>
       </c>
-      <c r="B97" s="22"/>
-      <c r="C97" s="21"/>
-      <c r="D97" s="18">
+      <c r="B97" s="21"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="17">
         <v>43938</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="18">
+      <c r="A98" s="17">
         <v>43940</v>
       </c>
-      <c r="B98" s="22"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="18">
+      <c r="B98" s="21"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="17">
         <v>43939</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="18">
+      <c r="A99" s="17">
         <v>43941</v>
       </c>
-      <c r="B99" s="22"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="18">
+      <c r="B99" s="21"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="17">
         <v>43940</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="18">
+      <c r="A100" s="17">
         <v>43942</v>
       </c>
-      <c r="B100" s="22"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="18">
+      <c r="B100" s="21"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="17">
         <v>43941</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="18">
+      <c r="A101" s="17">
         <v>43943</v>
       </c>
-      <c r="B101" s="22"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="18">
+      <c r="B101" s="21"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="17">
         <v>43942</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="18">
+      <c r="A102" s="17">
         <v>43944</v>
       </c>
-      <c r="B102" s="22"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="18">
+      <c r="B102" s="21"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="17">
         <v>43943</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="18">
+      <c r="A103" s="17">
         <v>43945</v>
       </c>
-      <c r="B103" s="22"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="18">
+      <c r="B103" s="21"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="17">
         <v>43944</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="18">
+      <c r="A104" s="17">
         <v>43946</v>
       </c>
-      <c r="B104" s="22"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="18">
+      <c r="B104" s="21"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="17">
         <v>43945</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="18">
+      <c r="A105" s="17">
         <v>43947</v>
       </c>
-      <c r="B105" s="22"/>
-      <c r="C105" s="21"/>
-      <c r="D105" s="18">
+      <c r="B105" s="21"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="17">
         <v>43946</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="18">
+      <c r="A106" s="17">
         <v>43948</v>
       </c>
-      <c r="B106" s="22"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="18">
+      <c r="B106" s="21"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="17">
         <v>43947</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="18">
+      <c r="A107" s="17">
         <v>43949</v>
       </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="18">
+      <c r="B107" s="21"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="17">
         <v>43948</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="18">
+      <c r="A108" s="17">
         <v>43950</v>
       </c>
-      <c r="B108" s="22"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="18">
+      <c r="B108" s="21"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="17">
         <v>43949</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="18">
+      <c r="A109" s="17">
         <v>43951</v>
       </c>
-      <c r="B109" s="22"/>
-      <c r="C109" s="21"/>
-      <c r="D109" s="18">
+      <c r="B109" s="21"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="17">
         <v>43950</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="18">
+      <c r="A110" s="17">
         <v>43952</v>
       </c>
-      <c r="B110" s="22"/>
-      <c r="C110" s="21"/>
-      <c r="D110" s="18">
+      <c r="B110" s="21"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="17">
         <v>43951</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="18">
+      <c r="A111" s="17">
         <v>43953</v>
       </c>
-      <c r="B111" s="22"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="18">
+      <c r="B111" s="21"/>
+      <c r="C111" s="20"/>
+      <c r="D111" s="17">
         <v>43952</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="18">
+      <c r="A112" s="17">
         <v>43954</v>
       </c>
-      <c r="B112" s="22"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="18">
+      <c r="B112" s="21"/>
+      <c r="C112" s="20"/>
+      <c r="D112" s="17">
         <v>43953</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="18">
+      <c r="A113" s="17">
         <v>43955</v>
       </c>
-      <c r="B113" s="22"/>
-      <c r="C113" s="21"/>
-      <c r="D113" s="18">
+      <c r="B113" s="21"/>
+      <c r="C113" s="20"/>
+      <c r="D113" s="17">
         <v>43954</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="18">
+      <c r="A114" s="17">
         <v>43956</v>
       </c>
-      <c r="B114" s="22"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="18">
+      <c r="B114" s="21"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="17">
         <v>43955</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="18">
+      <c r="A115" s="17">
         <v>43957</v>
       </c>
-      <c r="B115" s="22"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="18">
+      <c r="B115" s="21"/>
+      <c r="C115" s="20"/>
+      <c r="D115" s="17">
         <v>43956</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="18">
+      <c r="A116" s="17">
         <v>43958</v>
       </c>
-      <c r="B116" s="22"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="18">
+      <c r="B116" s="21"/>
+      <c r="C116" s="20"/>
+      <c r="D116" s="17">
         <v>43957</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="18">
+      <c r="A117" s="17">
         <v>43959</v>
       </c>
-      <c r="B117" s="22"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="18">
+      <c r="B117" s="21"/>
+      <c r="C117" s="20"/>
+      <c r="D117" s="17">
         <v>43958</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="18">
+      <c r="A118" s="17">
         <v>43960</v>
       </c>
-      <c r="B118" s="22"/>
-      <c r="C118" s="21"/>
-      <c r="D118" s="18">
+      <c r="B118" s="21"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="17">
         <v>43959</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="18">
+      <c r="A119" s="17">
         <v>43961</v>
       </c>
-      <c r="B119" s="22"/>
-      <c r="C119" s="21"/>
-      <c r="D119" s="18">
+      <c r="B119" s="21"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="17">
         <v>43960</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="18">
+      <c r="A120" s="17">
         <v>43962</v>
       </c>
-      <c r="B120" s="22"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="18">
+      <c r="B120" s="21"/>
+      <c r="C120" s="20"/>
+      <c r="D120" s="17">
         <v>43961</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="18">
+      <c r="A121" s="17">
         <v>43963</v>
       </c>
-      <c r="B121" s="22"/>
-      <c r="C121" s="21"/>
-      <c r="D121" s="18">
+      <c r="B121" s="21"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="17">
         <v>43962</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="18">
+      <c r="A122" s="17">
         <v>43964</v>
       </c>
-      <c r="B122" s="22"/>
-      <c r="C122" s="21"/>
-      <c r="D122" s="18">
+      <c r="B122" s="21"/>
+      <c r="C122" s="20"/>
+      <c r="D122" s="17">
         <v>43963</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="18">
+      <c r="A123" s="17">
         <v>43965</v>
       </c>
-      <c r="B123" s="22"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="18">
+      <c r="B123" s="21"/>
+      <c r="C123" s="20"/>
+      <c r="D123" s="17">
         <v>43964</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="18">
+      <c r="A124" s="17">
         <v>43966</v>
       </c>
-      <c r="B124" s="22"/>
-      <c r="C124" s="21"/>
-      <c r="D124" s="18">
+      <c r="B124" s="21"/>
+      <c r="C124" s="20"/>
+      <c r="D124" s="17">
         <v>43965</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="18">
+      <c r="A125" s="17">
         <v>43967</v>
       </c>
-      <c r="B125" s="22"/>
-      <c r="C125" s="21"/>
-      <c r="D125" s="18">
+      <c r="B125" s="21"/>
+      <c r="C125" s="20"/>
+      <c r="D125" s="17">
         <v>43966</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="18">
+      <c r="A126" s="17">
         <v>43968</v>
       </c>
-      <c r="B126" s="22"/>
-      <c r="C126" s="21"/>
-      <c r="D126" s="18">
+      <c r="B126" s="21"/>
+      <c r="C126" s="20"/>
+      <c r="D126" s="17">
         <v>43967</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="18">
+      <c r="A127" s="17">
         <v>43969</v>
       </c>
-      <c r="B127" s="22"/>
-      <c r="C127" s="21"/>
-      <c r="D127" s="18">
+      <c r="B127" s="21"/>
+      <c r="C127" s="20"/>
+      <c r="D127" s="17">
         <v>43968</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="18">
+      <c r="A128" s="17">
         <v>43970</v>
       </c>
-      <c r="B128" s="22"/>
-      <c r="C128" s="21"/>
-      <c r="D128" s="18">
+      <c r="B128" s="21"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="17">
         <v>43969</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="18">
+      <c r="A129" s="17">
         <v>43971</v>
       </c>
-      <c r="B129" s="22"/>
-      <c r="C129" s="21"/>
-      <c r="D129" s="18">
+      <c r="B129" s="21"/>
+      <c r="C129" s="20"/>
+      <c r="D129" s="17">
         <v>43970</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="18">
+      <c r="A130" s="17">
         <v>43972</v>
       </c>
-      <c r="B130" s="22"/>
-      <c r="C130" s="21"/>
-      <c r="D130" s="18">
+      <c r="B130" s="21"/>
+      <c r="C130" s="20"/>
+      <c r="D130" s="17">
         <v>43971</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="18">
+      <c r="A131" s="17">
         <v>43973</v>
       </c>
-      <c r="B131" s="22"/>
-      <c r="C131" s="21"/>
-      <c r="D131" s="18">
+      <c r="B131" s="21"/>
+      <c r="C131" s="20"/>
+      <c r="D131" s="17">
         <v>43972</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="18">
+      <c r="A132" s="17">
         <v>43974</v>
       </c>
-      <c r="B132" s="22"/>
-      <c r="C132" s="21"/>
-      <c r="D132" s="18">
+      <c r="B132" s="21"/>
+      <c r="C132" s="20"/>
+      <c r="D132" s="17">
         <v>43973</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="18">
+      <c r="A133" s="17">
         <v>43975</v>
       </c>
-      <c r="B133" s="22"/>
-      <c r="C133" s="21"/>
-      <c r="D133" s="18">
+      <c r="B133" s="21"/>
+      <c r="C133" s="20"/>
+      <c r="D133" s="17">
         <v>43974</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="18">
+      <c r="A134" s="17">
         <v>43976</v>
       </c>
-      <c r="B134" s="22"/>
-      <c r="C134" s="21"/>
-      <c r="D134" s="18">
+      <c r="B134" s="21"/>
+      <c r="C134" s="20"/>
+      <c r="D134" s="17">
         <v>43975</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="18">
+      <c r="A135" s="17">
         <v>43977</v>
       </c>
-      <c r="B135" s="22"/>
-      <c r="C135" s="21"/>
-      <c r="D135" s="18">
+      <c r="B135" s="21"/>
+      <c r="C135" s="20"/>
+      <c r="D135" s="17">
         <v>43976</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="18">
+      <c r="A136" s="17">
         <v>43978</v>
       </c>
-      <c r="B136" s="22"/>
-      <c r="C136" s="21"/>
-      <c r="D136" s="18">
+      <c r="B136" s="21"/>
+      <c r="C136" s="20"/>
+      <c r="D136" s="17">
         <v>43977</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="18">
+      <c r="A137" s="17">
         <v>43979</v>
       </c>
-      <c r="B137" s="22"/>
-      <c r="C137" s="21"/>
-      <c r="D137" s="18">
+      <c r="B137" s="21"/>
+      <c r="C137" s="20"/>
+      <c r="D137" s="17">
         <v>43978</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="18">
+      <c r="A138" s="17">
         <v>43980</v>
       </c>
-      <c r="B138" s="22"/>
-      <c r="C138" s="21"/>
-      <c r="D138" s="18">
+      <c r="B138" s="21"/>
+      <c r="C138" s="20"/>
+      <c r="D138" s="17">
         <v>43979</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="18">
+      <c r="A139" s="17">
         <v>43981</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="21"/>
-      <c r="D139" s="18">
+      <c r="B139" s="21"/>
+      <c r="C139" s="20"/>
+      <c r="D139" s="17">
         <v>43980</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="18">
+      <c r="A140" s="17">
         <v>43982</v>
       </c>
-      <c r="B140" s="22"/>
-      <c r="C140" s="21"/>
-      <c r="D140" s="18">
+      <c r="B140" s="21"/>
+      <c r="C140" s="20"/>
+      <c r="D140" s="17">
         <v>43981</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="18">
+      <c r="A141" s="17">
         <v>43983</v>
       </c>
-      <c r="B141" s="22"/>
-      <c r="C141" s="21"/>
-      <c r="D141" s="18">
+      <c r="B141" s="21"/>
+      <c r="C141" s="20"/>
+      <c r="D141" s="17">
         <v>43982</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="18">
+      <c r="A142" s="17">
         <v>43984</v>
       </c>
-      <c r="B142" s="22"/>
-      <c r="C142" s="21"/>
-      <c r="D142" s="18">
+      <c r="B142" s="21"/>
+      <c r="C142" s="20"/>
+      <c r="D142" s="17">
         <v>43983</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="18">
+      <c r="A143" s="17">
         <v>43985</v>
       </c>
-      <c r="B143" s="22"/>
-      <c r="C143" s="21"/>
-      <c r="D143" s="18">
+      <c r="B143" s="21"/>
+      <c r="C143" s="20"/>
+      <c r="D143" s="17">
         <v>43984</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="18">
+      <c r="A144" s="17">
         <v>43986</v>
       </c>
-      <c r="B144" s="22"/>
-      <c r="C144" s="21"/>
-      <c r="D144" s="18">
+      <c r="B144" s="21"/>
+      <c r="C144" s="20"/>
+      <c r="D144" s="17">
         <v>43985</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" s="18">
+      <c r="A145" s="17">
         <v>43987</v>
       </c>
-      <c r="B145" s="22"/>
-      <c r="C145" s="21"/>
-      <c r="D145" s="18">
+      <c r="B145" s="21"/>
+      <c r="C145" s="20"/>
+      <c r="D145" s="17">
         <v>43986</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" s="18">
+      <c r="A146" s="17">
         <v>43988</v>
       </c>
-      <c r="B146" s="22"/>
-      <c r="C146" s="21"/>
-      <c r="D146" s="18">
+      <c r="B146" s="21"/>
+      <c r="C146" s="20"/>
+      <c r="D146" s="17">
         <v>43987</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="18">
+      <c r="A147" s="17">
         <v>43989</v>
       </c>
-      <c r="B147" s="22"/>
-      <c r="C147" s="21"/>
-      <c r="D147" s="18">
+      <c r="B147" s="21"/>
+      <c r="C147" s="20"/>
+      <c r="D147" s="17">
         <v>43988</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" s="18">
+      <c r="A148" s="17">
         <v>43990</v>
       </c>
-      <c r="B148" s="22"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="18">
+      <c r="B148" s="21"/>
+      <c r="C148" s="20"/>
+      <c r="D148" s="17">
         <v>43989</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" s="18">
+      <c r="A149" s="17">
         <v>43991</v>
       </c>
-      <c r="B149" s="22"/>
-      <c r="C149" s="21"/>
-      <c r="D149" s="18">
+      <c r="B149" s="21"/>
+      <c r="C149" s="20"/>
+      <c r="D149" s="17">
         <v>43990</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="18">
+      <c r="A150" s="17">
         <v>43992</v>
       </c>
-      <c r="B150" s="22"/>
-      <c r="C150" s="21"/>
-      <c r="D150" s="18">
+      <c r="B150" s="21"/>
+      <c r="C150" s="20"/>
+      <c r="D150" s="17">
         <v>43991</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A151" s="18">
+      <c r="A151" s="17">
         <v>43993</v>
       </c>
-      <c r="B151" s="22"/>
-      <c r="C151" s="21"/>
-      <c r="D151" s="18">
+      <c r="B151" s="21"/>
+      <c r="C151" s="20"/>
+      <c r="D151" s="17">
         <v>43992</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A152" s="18">
+      <c r="A152" s="17">
         <v>43994</v>
       </c>
-      <c r="B152" s="22"/>
-      <c r="C152" s="21"/>
-      <c r="D152" s="18">
+      <c r="B152" s="21"/>
+      <c r="C152" s="20"/>
+      <c r="D152" s="17">
         <v>43993</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" s="18">
+      <c r="A153" s="17">
         <v>43995</v>
       </c>
-      <c r="B153" s="22"/>
-      <c r="C153" s="21"/>
-      <c r="D153" s="18">
+      <c r="B153" s="21"/>
+      <c r="C153" s="20"/>
+      <c r="D153" s="17">
         <v>43994</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" s="18">
+      <c r="A154" s="17">
         <v>43996</v>
       </c>
-      <c r="B154" s="22"/>
-      <c r="C154" s="21"/>
-      <c r="D154" s="18">
+      <c r="B154" s="21"/>
+      <c r="C154" s="20"/>
+      <c r="D154" s="17">
         <v>43995</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A155" s="18">
+      <c r="A155" s="17">
         <v>43997</v>
       </c>
-      <c r="B155" s="22"/>
-      <c r="C155" s="21"/>
-      <c r="D155" s="18">
+      <c r="B155" s="21"/>
+      <c r="C155" s="20"/>
+      <c r="D155" s="17">
         <v>43996</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A156" s="19"/>
-      <c r="D156" s="18">
+      <c r="A156" s="18"/>
+      <c r="D156" s="17">
         <v>43997</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A157" s="19"/>
-      <c r="D157" s="19"/>
+      <c r="A157" s="18"/>
+      <c r="D157" s="18"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A158" s="19"/>
-      <c r="D158" s="19"/>
+      <c r="A158" s="18"/>
+      <c r="D158" s="18"/>
     </row>
     <row r="159" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="10" t="s">
+      <c r="A159" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C159" s="12">
+      <c r="C159" s="11">
         <f>SUM(C64:C155)</f>
-        <v>21</v>
-      </c>
-      <c r="D159" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D159" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F159" s="5">
+      <c r="F159" s="11">
         <f>SUM(F65:F156)</f>
         <v>29</v>
       </c>
-      <c r="I159" s="6">
+      <c r="I159" s="5">
         <f>SUM(I2:I155)</f>
         <v>0</v>
       </c>
-      <c r="L159" s="6">
+      <c r="L159" s="5">
         <f>SUM(L2:L155)</f>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D160" s="10"/>
+      <c r="D160" s="9"/>
     </row>
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Uptade Thomas journal d'activité
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal d'activité.xlsx
+++ b/Journal d'activité/Journal d'activité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AE5E9B-C235-4050-84BF-CA00BB4CB18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F652CE4-A63B-402A-8FD3-8127503C47CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -349,7 +349,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -414,12 +414,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -470,6 +473,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -792,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,55 +833,55 @@
       <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="37"/>
+      <c r="G1" s="38"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="39"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-      <c r="M1" s="26"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="13"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="40"/>
+      <c r="J2" s="41"/>
       <c r="K2" s="13"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="27"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="17">
         <v>43845</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="30"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
@@ -882,25 +891,25 @@
       <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="17">
         <v>43846</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="17">
         <v>43847</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
@@ -910,49 +919,49 @@
       <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="17">
         <v>43848</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="17">
         <v>43849</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="17">
         <v>43850</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="17">
         <v>43851</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
@@ -962,13 +971,13 @@
       <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="17">
         <v>43852</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
@@ -978,73 +987,73 @@
       <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="17">
         <v>43853</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="17">
         <v>43854</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="17">
         <v>43855</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="17">
         <v>43856</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="17">
         <v>43857</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="17">
         <v>43858</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
@@ -1054,13 +1063,13 @@
       <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="17">
         <v>43859</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
@@ -1070,25 +1079,25 @@
       <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="17">
         <v>43860</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="17">
         <v>43861</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
@@ -1096,49 +1105,49 @@
       <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="17">
         <v>43862</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="17">
         <v>43863</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="17">
         <v>43864</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="17">
         <v>43865</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
@@ -1148,13 +1157,13 @@
       <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="17">
         <v>43866</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
@@ -1164,25 +1173,25 @@
       <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="17">
         <v>43867</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="17">
         <v>43868</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
@@ -1192,49 +1201,49 @@
       <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="17">
         <v>43869</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="17">
         <v>43870</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="17">
         <v>43871</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
       <c r="D30" s="17">
         <v>43872</v>
       </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
@@ -1244,13 +1253,13 @@
       <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
       <c r="D31" s="17">
         <v>43873</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
@@ -1260,25 +1269,25 @@
       <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="17">
         <v>43874</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="17">
         <v>43875</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
@@ -1288,145 +1297,145 @@
       <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="17">
         <v>43876</v>
       </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="17">
         <v>43877</v>
       </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="17">
         <v>43878</v>
       </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="17">
         <v>43879</v>
       </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="17">
         <v>43880</v>
       </c>
-      <c r="E38" s="30"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="17">
         <v>43881</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="17">
         <v>43882</v>
       </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="17">
         <v>43883</v>
       </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="32"/>
       <c r="D42" s="17">
         <v>43884</v>
       </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
       <c r="D43" s="17">
         <v>43885</v>
       </c>
-      <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="32"/>
       <c r="D44" s="17">
         <v>43886</v>
       </c>
-      <c r="E44" s="30"/>
-      <c r="F44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="32"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="17">
         <v>43887</v>
       </c>
-      <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="32"/>
       <c r="H45" s="4"/>
       <c r="K45" s="4"/>
     </row>
@@ -1434,73 +1443,73 @@
       <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="31"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="17">
         <v>43888</v>
       </c>
-      <c r="E46" s="30"/>
-      <c r="F46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="32"/>
       <c r="D47" s="17">
         <v>43889</v>
       </c>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="30"/>
-      <c r="C48" s="31"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
       <c r="D48" s="17">
         <v>43890</v>
       </c>
-      <c r="E48" s="30"/>
-      <c r="F48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="32"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="31"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="32"/>
       <c r="D49" s="17">
         <v>43891</v>
       </c>
-      <c r="E49" s="30"/>
-      <c r="F49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="32"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="31"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="17">
         <v>43892</v>
       </c>
-      <c r="E50" s="30"/>
-      <c r="F50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="32"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="31"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="17">
         <v>43893</v>
       </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="32"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
       <c r="K51" s="4"/>
@@ -1510,13 +1519,13 @@
       <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="32"/>
       <c r="D52" s="17">
         <v>43894</v>
       </c>
-      <c r="E52" s="30"/>
-      <c r="F52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="32"/>
       <c r="H52" s="4"/>
       <c r="I52" s="1"/>
       <c r="K52" s="4"/>
@@ -1526,25 +1535,25 @@
       <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="31"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="32"/>
       <c r="D53" s="17">
         <v>43895</v>
       </c>
-      <c r="E53" s="30"/>
-      <c r="F53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="32"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="32"/>
       <c r="D54" s="17">
         <v>43896</v>
       </c>
-      <c r="E54" s="30"/>
-      <c r="F54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="32"/>
       <c r="H54" s="4"/>
       <c r="I54" s="1"/>
       <c r="K54" s="4"/>
@@ -1554,49 +1563,49 @@
       <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="32"/>
       <c r="D55" s="17">
         <v>43897</v>
       </c>
-      <c r="E55" s="30"/>
-      <c r="F55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="30"/>
-      <c r="C56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="32"/>
       <c r="D56" s="17">
         <v>43898</v>
       </c>
-      <c r="E56" s="30"/>
-      <c r="F56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32"/>
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="30"/>
-      <c r="C57" s="31"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="32"/>
       <c r="D57" s="17">
         <v>43899</v>
       </c>
-      <c r="E57" s="30"/>
-      <c r="F57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="30"/>
-      <c r="C58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="32"/>
       <c r="D58" s="17">
         <v>43900</v>
       </c>
-      <c r="E58" s="30"/>
-      <c r="F58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="32"/>
       <c r="H58" s="4"/>
       <c r="I58" s="1"/>
       <c r="K58" s="4"/>
@@ -1606,13 +1615,13 @@
       <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="32"/>
       <c r="D59" s="17">
         <v>43901</v>
       </c>
-      <c r="E59" s="30"/>
-      <c r="F59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="32"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="K59" s="4"/>
@@ -1622,25 +1631,25 @@
       <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="30"/>
-      <c r="C60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="32"/>
       <c r="D60" s="17">
         <v>43902</v>
       </c>
-      <c r="E60" s="30"/>
-      <c r="F60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="32"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="32"/>
       <c r="D61" s="17">
         <v>43903</v>
       </c>
-      <c r="E61" s="30"/>
-      <c r="F61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="32"/>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="K61" s="4"/>
@@ -1650,25 +1659,25 @@
       <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="30"/>
-      <c r="C62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="32"/>
       <c r="D62" s="17">
         <v>43904</v>
       </c>
-      <c r="E62" s="30"/>
-      <c r="F62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="32"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="32"/>
       <c r="D63" s="17">
         <v>43905</v>
       </c>
-      <c r="E63" s="30"/>
-      <c r="F63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="32"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -1683,31 +1692,35 @@
       <c r="D64" s="17">
         <v>43906</v>
       </c>
-      <c r="E64" s="30"/>
-      <c r="F64" s="31"/>
+      <c r="E64" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="24">
+        <v>2</v>
+      </c>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
       <c r="K64" s="4"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B65" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="33">
+      <c r="C65" s="34">
         <v>10</v>
       </c>
       <c r="D65" s="17">
         <v>43907</v>
       </c>
-      <c r="E65" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" s="22">
-        <v>2</v>
+      <c r="E65" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="34">
+        <v>13</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="1"/>
@@ -1718,17 +1731,13 @@
       <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="33"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="34"/>
       <c r="D66" s="17">
         <v>43908</v>
       </c>
-      <c r="E66" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F66" s="33">
-        <v>13</v>
-      </c>
+      <c r="E66" s="33"/>
+      <c r="F66" s="34"/>
       <c r="H66" s="4"/>
       <c r="I66" s="1"/>
       <c r="K66" s="4"/>
@@ -1738,13 +1747,13 @@
       <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="33"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="17">
         <v>43909</v>
       </c>
-      <c r="E67" s="32"/>
-      <c r="F67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="34"/>
       <c r="H67" s="4"/>
       <c r="I67" s="1"/>
       <c r="K67" s="4"/>
@@ -1754,45 +1763,45 @@
       <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="33"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="34"/>
       <c r="D68" s="17">
         <v>43910</v>
       </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="34"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="32" t="s">
+      <c r="B69" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="34">
+      <c r="C69" s="35">
         <v>4</v>
       </c>
       <c r="D69" s="17">
         <v>43911</v>
       </c>
-      <c r="E69" s="32"/>
-      <c r="F69" s="33"/>
+      <c r="E69" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="26">
+        <v>8</v>
+      </c>
     </row>
     <row r="70" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="34"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="35"/>
       <c r="D70" s="17">
         <v>43912</v>
       </c>
-      <c r="E70" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="25">
-        <v>8</v>
-      </c>
+      <c r="E70" s="33"/>
+      <c r="F70" s="26"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
@@ -1807,10 +1816,14 @@
       <c r="D71" s="17">
         <v>43913</v>
       </c>
-      <c r="E71" s="32"/>
-      <c r="F71" s="25"/>
-    </row>
-    <row r="72" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E71" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>43914</v>
       </c>
@@ -1823,12 +1836,8 @@
       <c r="D72" s="17">
         <v>43914</v>
       </c>
-      <c r="E72" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F72" s="25">
-        <v>6</v>
-      </c>
+      <c r="E72" s="25"/>
+      <c r="F72" s="26"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
@@ -1843,8 +1852,8 @@
       <c r="D73" s="17">
         <v>43915</v>
       </c>
-      <c r="E73" s="24"/>
-      <c r="F73" s="25"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="42"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
@@ -2691,7 +2700,7 @@
       </c>
       <c r="F159" s="11">
         <f>SUM(F65:F156)</f>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I159" s="5">
         <f>SUM(I2:I155)</f>
@@ -2708,22 +2717,22 @@
     <row r="161" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E3:F63"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="B2:C63"/>
     <mergeCell ref="B65:B68"/>
     <mergeCell ref="C65:C68"/>
-    <mergeCell ref="E3:F64"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="E66:E69"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="E70:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
maj bdd et JA
</commit_message>
<xml_diff>
--- a/Journal d'activité/Journal d'activité.xlsx
+++ b/Journal d'activité/Journal d'activité.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinne\OneDrive\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CORENTIN1\Documents\GitHub\Systeme_Escape_Game_13emePorte\Journal d'activité\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDC3585-711F-4481-995E-1995E9258CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F83452-C887-47CF-97EB-A4FB2D543FD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28170" windowHeight="15360" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -63,6 +63,45 @@
   </si>
   <si>
     <t>Travail sur un tutoriel de la configuratrion IP fixe pour la société 13ème Porte</t>
+  </si>
+  <si>
+    <t>BRENY Corentin</t>
+  </si>
+  <si>
+    <t>NB Heures</t>
+  </si>
+  <si>
+    <t>Organisation du groupe</t>
+  </si>
+  <si>
+    <t>Travail sur la base de données, réflexion comment procéder. Installation Wampserver.</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>Week-end</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Correction de la BDD transmise par le prof. Organisation pour l'accès des autres à la bdd.</t>
+  </si>
+  <si>
+    <t>Résolution problème PhpMyAdmin. Modification de la BDD sur excel.</t>
+  </si>
+  <si>
+    <t>Création de la BDD sur PhpMyAdmin.</t>
+  </si>
+  <si>
+    <t>MAJ du Journal D'Activité</t>
   </si>
 </sst>
 </file>
@@ -320,7 +359,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,9 +370,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -364,16 +400,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -394,6 +424,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,20 +466,32 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -760,1358 +814,1468 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:M160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="22"/>
+    <col min="1" max="1" width="11.42578125" style="19"/>
     <col min="2" max="2" width="49.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="9"/>
-    <col min="5" max="5" width="44.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="9"/>
+    <col min="4" max="4" width="11.42578125" style="8"/>
+    <col min="5" max="5" width="44.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="8"/>
     <col min="8" max="8" width="42.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="10"/>
+    <col min="10" max="10" width="11.42578125" style="9"/>
     <col min="11" max="11" width="34.42578125" style="2" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="9" customWidth="1"/>
     <col min="14" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="29"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="17">
         <v>43844</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="A3" s="17">
         <v>43845</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="38"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="K3" s="3"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="17">
         <v>43846</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="17">
         <v>43847</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="38"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="17">
         <v>43848</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="17">
         <v>43849</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="17">
         <v>43850</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="17">
         <v>43851</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="38"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="K9" s="3"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="17">
         <v>43852</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="38"/>
       <c r="H10" s="3"/>
       <c r="I10" s="1"/>
       <c r="K10" s="3"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="A11" s="17">
         <v>43853</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="A12" s="17">
         <v>43854</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="A13" s="17">
         <v>43855</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="17">
         <v>43856</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="A15" s="17">
         <v>43857</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="A16" s="17">
         <v>43858</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="38"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="K16" s="3"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="17">
         <v>43859</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="38"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
       <c r="K17" s="3"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="17">
         <v>43860</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="17">
         <v>43861</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="38"/>
       <c r="I19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="17">
         <v>43862</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="A21" s="17">
         <v>43863</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="A22" s="17">
         <v>43864</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="E22" s="3"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="A23" s="17">
         <v>43865</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="38"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1"/>
       <c r="K23" s="3"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
+      <c r="A24" s="17">
         <v>43866</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="38"/>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
       <c r="K24" s="3"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
+      <c r="A25" s="17">
         <v>43867</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="E25" s="3"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
+      <c r="A26" s="17">
         <v>43868</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="38"/>
       <c r="H26" s="3"/>
       <c r="I26" s="1"/>
       <c r="K26" s="3"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
+      <c r="A27" s="17">
         <v>43869</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="E27" s="3"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
+      <c r="A28" s="17">
         <v>43870</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="E28" s="3"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
+      <c r="A29" s="17">
         <v>43871</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="E29" s="3"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
+      <c r="A30" s="17">
         <v>43872</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="38"/>
       <c r="H30" s="3"/>
       <c r="I30" s="1"/>
       <c r="K30" s="3"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
+      <c r="A31" s="17">
         <v>43873</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="34"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="38"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
       <c r="K31" s="3"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
+      <c r="A32" s="17">
         <v>43874</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34"/>
-      <c r="E32" s="3"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
+      <c r="A33" s="17">
         <v>43875</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="38"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
       <c r="K33" s="3"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
+      <c r="A34" s="17">
         <v>43876</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
-      <c r="E34" s="3"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="38"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
+      <c r="A35" s="17">
         <v>43877</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-      <c r="E35" s="3"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
+      <c r="A36" s="17">
         <v>43878</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="34"/>
-      <c r="E36" s="3"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
+      <c r="A37" s="17">
         <v>43879</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="34"/>
-      <c r="E37" s="3"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="38"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
+      <c r="A38" s="17">
         <v>43880</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="34"/>
-      <c r="E38" s="3"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="38"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="20">
+      <c r="A39" s="17">
         <v>43881</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
-      <c r="E39" s="3"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="38"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="20">
+      <c r="A40" s="17">
         <v>43882</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
-      <c r="E40" s="3"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="38"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
+      <c r="A41" s="17">
         <v>43883</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="34"/>
-      <c r="E41" s="3"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="35"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="38"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
+      <c r="A42" s="17">
         <v>43884</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="34"/>
-      <c r="E42" s="3"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="38"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="20">
+      <c r="A43" s="17">
         <v>43885</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="34"/>
-      <c r="E43" s="3"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="38"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
+      <c r="A44" s="17">
         <v>43886</v>
       </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="34"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="35"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="38"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
+      <c r="A45" s="17">
         <v>43887</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="34"/>
-      <c r="F45" s="4"/>
-      <c r="H45" s="5"/>
-      <c r="K45" s="5"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="38"/>
+      <c r="H45" s="4"/>
+      <c r="K45" s="4"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
+      <c r="A46" s="17">
         <v>43888</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="38"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
+      <c r="A47" s="17">
         <v>43889</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="35"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="38"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="20">
+      <c r="A48" s="17">
         <v>43890</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="35"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="38"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="20">
+      <c r="A49" s="17">
         <v>43891</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="38"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
+      <c r="A50" s="17">
         <v>43892</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="38"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="20">
+      <c r="A51" s="17">
         <v>43893</v>
       </c>
-      <c r="B51" s="33"/>
-      <c r="C51" s="34"/>
-      <c r="F51" s="4"/>
-      <c r="H51" s="5"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="35"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="38"/>
+      <c r="H51" s="4"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="5"/>
+      <c r="K51" s="4"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="20">
+      <c r="A52" s="17">
         <v>43894</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="34"/>
-      <c r="F52" s="4"/>
-      <c r="H52" s="5"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="35"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="38"/>
+      <c r="H52" s="4"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="5"/>
+      <c r="K52" s="4"/>
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="20">
+      <c r="A53" s="17">
         <v>43895</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="38"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
+      <c r="A54" s="17">
         <v>43896</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="34"/>
-      <c r="F54" s="4"/>
-      <c r="H54" s="5"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="35"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="38"/>
+      <c r="H54" s="4"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="5"/>
+      <c r="K54" s="4"/>
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
+      <c r="A55" s="17">
         <v>43897</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="34"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="38"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="20">
+      <c r="A56" s="17">
         <v>43898</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="38"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="20">
+      <c r="A57" s="17">
         <v>43899</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="38"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="20">
+      <c r="A58" s="17">
         <v>43900</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="34"/>
-      <c r="F58" s="4"/>
-      <c r="H58" s="5"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="38"/>
+      <c r="H58" s="4"/>
       <c r="I58" s="1"/>
-      <c r="K58" s="5"/>
+      <c r="K58" s="4"/>
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="20">
+      <c r="A59" s="17">
         <v>43901</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="34"/>
-      <c r="F59" s="4"/>
-      <c r="H59" s="5"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="35"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="38"/>
+      <c r="H59" s="4"/>
       <c r="I59" s="1"/>
-      <c r="K59" s="5"/>
+      <c r="K59" s="4"/>
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
+      <c r="A60" s="17">
         <v>43902</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="35"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="38"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="20">
+      <c r="A61" s="17">
         <v>43903</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="34"/>
-      <c r="F61" s="4"/>
-      <c r="H61" s="5"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="38"/>
+      <c r="H61" s="4"/>
       <c r="I61" s="1"/>
-      <c r="K61" s="5"/>
+      <c r="K61" s="4"/>
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
+      <c r="A62" s="17">
         <v>43904</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="C62" s="34"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="35"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="38"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="20">
+      <c r="A63" s="17">
         <v>43905</v>
       </c>
-      <c r="B63" s="33"/>
-      <c r="C63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="35"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="38"/>
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20">
+      <c r="A64" s="17">
         <v>43906</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="23">
+      <c r="C64" s="20">
         <v>2</v>
       </c>
-      <c r="F64" s="4"/>
-      <c r="H64" s="5"/>
+      <c r="E64" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="4"/>
       <c r="I64" s="1"/>
-      <c r="K64" s="5"/>
+      <c r="K64" s="4"/>
       <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="20">
+      <c r="A65" s="17">
         <v>43907</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="36">
         <v>10</v>
       </c>
-      <c r="F65" s="4"/>
-      <c r="H65" s="5"/>
+      <c r="E65" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" s="4"/>
       <c r="I65" s="1"/>
-      <c r="K65" s="5"/>
+      <c r="K65" s="4"/>
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="20">
+      <c r="A66" s="17">
         <v>43908</v>
       </c>
-      <c r="B66" s="35"/>
+      <c r="B66" s="22"/>
       <c r="C66" s="36"/>
-      <c r="F66" s="4"/>
-      <c r="H66" s="5"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="43"/>
+      <c r="H66" s="4"/>
       <c r="I66" s="1"/>
-      <c r="K66" s="5"/>
+      <c r="K66" s="4"/>
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="20">
+      <c r="A67" s="17">
         <v>43909</v>
       </c>
-      <c r="B67" s="35"/>
+      <c r="B67" s="22"/>
       <c r="C67" s="36"/>
-      <c r="F67" s="4"/>
-      <c r="H67" s="5"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="43"/>
+      <c r="H67" s="4"/>
       <c r="I67" s="1"/>
-      <c r="K67" s="5"/>
+      <c r="K67" s="4"/>
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="20">
+      <c r="A68" s="17">
         <v>43910</v>
       </c>
-      <c r="B68" s="35"/>
+      <c r="B68" s="22"/>
       <c r="C68" s="36"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="20">
+      <c r="A69" s="17">
         <v>43911</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="37">
+      <c r="C69" s="23">
         <v>4</v>
       </c>
+      <c r="E69" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" s="44"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="20">
+      <c r="A70" s="17">
         <v>43912</v>
       </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="37"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="44"/>
     </row>
     <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="20">
+      <c r="A71" s="17">
         <v>43913</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="23">
+      <c r="C71" s="20">
         <v>2</v>
       </c>
+      <c r="E71" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="72" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
+      <c r="A72" s="17">
         <v>43914</v>
       </c>
-      <c r="B72" s="24" t="s">
+      <c r="B72" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="23">
+      <c r="C72" s="20">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="20">
+      <c r="E72" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="17">
         <v>43915</v>
       </c>
-      <c r="B73" s="24"/>
-      <c r="C73" s="23"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="20"/>
+      <c r="E73" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="20">
+      <c r="A74" s="17">
         <v>43916</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="23"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="20"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="20">
+      <c r="A75" s="17">
         <v>43917</v>
       </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="23"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="20"/>
+      <c r="E75" s="21" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="20">
+      <c r="A76" s="17">
         <v>43918</v>
       </c>
-      <c r="B76" s="24"/>
-      <c r="C76" s="23"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="20"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="20">
+      <c r="A77" s="17">
         <v>43919</v>
       </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="23"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="20"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="20">
+      <c r="A78" s="17">
         <v>43920</v>
       </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="23"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="20"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="20">
+      <c r="A79" s="17">
         <v>43921</v>
       </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="23"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="20"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="20">
+      <c r="A80" s="17">
         <v>43922</v>
       </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="23"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="20"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="20">
+      <c r="A81" s="17">
         <v>43923</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="23"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="20"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="20">
+      <c r="A82" s="17">
         <v>43924</v>
       </c>
-      <c r="B82" s="24"/>
-      <c r="C82" s="23"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="20"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="20">
+      <c r="A83" s="17">
         <v>43925</v>
       </c>
-      <c r="B83" s="24"/>
-      <c r="C83" s="23"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="20"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="20">
+      <c r="A84" s="17">
         <v>43926</v>
       </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="23"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="20"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="20">
+      <c r="A85" s="17">
         <v>43927</v>
       </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="23"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="20"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="20">
+      <c r="A86" s="17">
         <v>43928</v>
       </c>
-      <c r="B86" s="24"/>
-      <c r="C86" s="23"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="20"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="20">
+      <c r="A87" s="17">
         <v>43929</v>
       </c>
-      <c r="B87" s="24"/>
-      <c r="C87" s="23"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="20"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="20">
+      <c r="A88" s="17">
         <v>43930</v>
       </c>
-      <c r="B88" s="24"/>
-      <c r="C88" s="23"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="20"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="20">
+      <c r="A89" s="17">
         <v>43931</v>
       </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="23"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="20"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="20">
+      <c r="A90" s="17">
         <v>43932</v>
       </c>
-      <c r="B90" s="24"/>
-      <c r="C90" s="23"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="20"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="20">
+      <c r="A91" s="17">
         <v>43933</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="23"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="20"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="20">
+      <c r="A92" s="17">
         <v>43934</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="23"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="20"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="20">
+      <c r="A93" s="17">
         <v>43935</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="23"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="20"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="20">
+      <c r="A94" s="17">
         <v>43936</v>
       </c>
-      <c r="B94" s="24"/>
-      <c r="C94" s="23"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="20"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="20">
+      <c r="A95" s="17">
         <v>43937</v>
       </c>
-      <c r="B95" s="24"/>
-      <c r="C95" s="23"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="20"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="20">
+      <c r="A96" s="17">
         <v>43938</v>
       </c>
-      <c r="B96" s="24"/>
-      <c r="C96" s="23"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="20"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="20">
+      <c r="A97" s="17">
         <v>43939</v>
       </c>
-      <c r="B97" s="24"/>
-      <c r="C97" s="23"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="20"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="20">
+      <c r="A98" s="17">
         <v>43940</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="23"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="20"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="20">
+      <c r="A99" s="17">
         <v>43941</v>
       </c>
-      <c r="B99" s="24"/>
-      <c r="C99" s="23"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="20"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="20">
+      <c r="A100" s="17">
         <v>43942</v>
       </c>
-      <c r="B100" s="24"/>
-      <c r="C100" s="23"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="20"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="20">
+      <c r="A101" s="17">
         <v>43943</v>
       </c>
-      <c r="B101" s="24"/>
-      <c r="C101" s="23"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="20">
+      <c r="A102" s="17">
         <v>43944</v>
       </c>
-      <c r="B102" s="24"/>
-      <c r="C102" s="23"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="20"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="20">
+      <c r="A103" s="17">
         <v>43945</v>
       </c>
-      <c r="B103" s="24"/>
-      <c r="C103" s="23"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="20"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="20">
+      <c r="A104" s="17">
         <v>43946</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="23"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="20"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="20">
+      <c r="A105" s="17">
         <v>43947</v>
       </c>
-      <c r="B105" s="24"/>
-      <c r="C105" s="23"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="20"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="20">
+      <c r="A106" s="17">
         <v>43948</v>
       </c>
-      <c r="B106" s="24"/>
-      <c r="C106" s="23"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="20"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="20">
+      <c r="A107" s="17">
         <v>43949</v>
       </c>
-      <c r="B107" s="24"/>
-      <c r="C107" s="23"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="20"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="20">
+      <c r="A108" s="17">
         <v>43950</v>
       </c>
-      <c r="B108" s="24"/>
-      <c r="C108" s="23"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="20"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="20">
+      <c r="A109" s="17">
         <v>43951</v>
       </c>
-      <c r="B109" s="24"/>
-      <c r="C109" s="23"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="20"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="20">
+      <c r="A110" s="17">
         <v>43952</v>
       </c>
-      <c r="B110" s="24"/>
-      <c r="C110" s="23"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="20"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="20">
+      <c r="A111" s="17">
         <v>43953</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="23"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="20"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="20">
+      <c r="A112" s="17">
         <v>43954</v>
       </c>
-      <c r="B112" s="24"/>
-      <c r="C112" s="23"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="20"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="20">
+      <c r="A113" s="17">
         <v>43955</v>
       </c>
-      <c r="B113" s="24"/>
-      <c r="C113" s="23"/>
+      <c r="B113" s="21"/>
+      <c r="C113" s="20"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="20">
+      <c r="A114" s="17">
         <v>43956</v>
       </c>
-      <c r="B114" s="24"/>
-      <c r="C114" s="23"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="20"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="20">
+      <c r="A115" s="17">
         <v>43957</v>
       </c>
-      <c r="B115" s="24"/>
-      <c r="C115" s="23"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="20"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="20">
+      <c r="A116" s="17">
         <v>43958</v>
       </c>
-      <c r="B116" s="24"/>
-      <c r="C116" s="23"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="20"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="20">
+      <c r="A117" s="17">
         <v>43959</v>
       </c>
-      <c r="B117" s="24"/>
-      <c r="C117" s="23"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="20"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="20">
+      <c r="A118" s="17">
         <v>43960</v>
       </c>
-      <c r="B118" s="24"/>
-      <c r="C118" s="23"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="20"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="20">
+      <c r="A119" s="17">
         <v>43961</v>
       </c>
-      <c r="B119" s="24"/>
-      <c r="C119" s="23"/>
+      <c r="B119" s="21"/>
+      <c r="C119" s="20"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="20">
+      <c r="A120" s="17">
         <v>43962</v>
       </c>
-      <c r="B120" s="24"/>
-      <c r="C120" s="23"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="20"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="20">
+      <c r="A121" s="17">
         <v>43963</v>
       </c>
-      <c r="B121" s="24"/>
-      <c r="C121" s="23"/>
+      <c r="B121" s="21"/>
+      <c r="C121" s="20"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="20">
+      <c r="A122" s="17">
         <v>43964</v>
       </c>
-      <c r="B122" s="24"/>
-      <c r="C122" s="23"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="20"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="20">
+      <c r="A123" s="17">
         <v>43965</v>
       </c>
-      <c r="B123" s="24"/>
-      <c r="C123" s="23"/>
+      <c r="B123" s="21"/>
+      <c r="C123" s="20"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="20">
+      <c r="A124" s="17">
         <v>43966</v>
       </c>
-      <c r="B124" s="24"/>
-      <c r="C124" s="23"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="20"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="20">
+      <c r="A125" s="17">
         <v>43967</v>
       </c>
-      <c r="B125" s="24"/>
-      <c r="C125" s="23"/>
+      <c r="B125" s="21"/>
+      <c r="C125" s="20"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="20">
+      <c r="A126" s="17">
         <v>43968</v>
       </c>
-      <c r="B126" s="24"/>
-      <c r="C126" s="23"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="20"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="20">
+      <c r="A127" s="17">
         <v>43969</v>
       </c>
-      <c r="B127" s="24"/>
-      <c r="C127" s="23"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="20"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="20">
+      <c r="A128" s="17">
         <v>43970</v>
       </c>
-      <c r="B128" s="24"/>
-      <c r="C128" s="23"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="20"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="20">
+      <c r="A129" s="17">
         <v>43971</v>
       </c>
-      <c r="B129" s="24"/>
-      <c r="C129" s="23"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="20"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="20">
+      <c r="A130" s="17">
         <v>43972</v>
       </c>
-      <c r="B130" s="24"/>
-      <c r="C130" s="23"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="20"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="20">
+      <c r="A131" s="17">
         <v>43973</v>
       </c>
-      <c r="B131" s="24"/>
-      <c r="C131" s="23"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="20"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="20">
+      <c r="A132" s="17">
         <v>43974</v>
       </c>
-      <c r="B132" s="24"/>
-      <c r="C132" s="23"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="20"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="20">
+      <c r="A133" s="17">
         <v>43975</v>
       </c>
-      <c r="B133" s="24"/>
-      <c r="C133" s="23"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="20"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="20">
+      <c r="A134" s="17">
         <v>43976</v>
       </c>
-      <c r="B134" s="24"/>
-      <c r="C134" s="23"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="20"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="20">
+      <c r="A135" s="17">
         <v>43977</v>
       </c>
-      <c r="B135" s="24"/>
-      <c r="C135" s="23"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="20"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="20">
+      <c r="A136" s="17">
         <v>43978</v>
       </c>
-      <c r="B136" s="24"/>
-      <c r="C136" s="23"/>
+      <c r="B136" s="21"/>
+      <c r="C136" s="20"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="20">
+      <c r="A137" s="17">
         <v>43979</v>
       </c>
-      <c r="B137" s="24"/>
-      <c r="C137" s="23"/>
+      <c r="B137" s="21"/>
+      <c r="C137" s="20"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="20">
+      <c r="A138" s="17">
         <v>43980</v>
       </c>
-      <c r="B138" s="24"/>
-      <c r="C138" s="23"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="20"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="20">
+      <c r="A139" s="17">
         <v>43981</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="21"/>
+      <c r="C139" s="20"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="20">
+      <c r="A140" s="17">
         <v>43982</v>
       </c>
-      <c r="B140" s="24"/>
-      <c r="C140" s="23"/>
+      <c r="B140" s="21"/>
+      <c r="C140" s="20"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="20">
+      <c r="A141" s="17">
         <v>43983</v>
       </c>
-      <c r="B141" s="24"/>
-      <c r="C141" s="23"/>
+      <c r="B141" s="21"/>
+      <c r="C141" s="20"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="20">
+      <c r="A142" s="17">
         <v>43984</v>
       </c>
-      <c r="B142" s="24"/>
-      <c r="C142" s="23"/>
+      <c r="B142" s="21"/>
+      <c r="C142" s="20"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="20">
+      <c r="A143" s="17">
         <v>43985</v>
       </c>
-      <c r="B143" s="24"/>
-      <c r="C143" s="23"/>
+      <c r="B143" s="21"/>
+      <c r="C143" s="20"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="20">
+      <c r="A144" s="17">
         <v>43986</v>
       </c>
-      <c r="B144" s="24"/>
-      <c r="C144" s="23"/>
+      <c r="B144" s="21"/>
+      <c r="C144" s="20"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" s="20">
+      <c r="A145" s="17">
         <v>43987</v>
       </c>
-      <c r="B145" s="24"/>
-      <c r="C145" s="23"/>
+      <c r="B145" s="21"/>
+      <c r="C145" s="20"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" s="20">
+      <c r="A146" s="17">
         <v>43988</v>
       </c>
-      <c r="B146" s="24"/>
-      <c r="C146" s="23"/>
+      <c r="B146" s="21"/>
+      <c r="C146" s="20"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="20">
+      <c r="A147" s="17">
         <v>43989</v>
       </c>
-      <c r="B147" s="24"/>
-      <c r="C147" s="23"/>
+      <c r="B147" s="21"/>
+      <c r="C147" s="20"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" s="20">
+      <c r="A148" s="17">
         <v>43990</v>
       </c>
-      <c r="B148" s="24"/>
-      <c r="C148" s="23"/>
+      <c r="B148" s="21"/>
+      <c r="C148" s="20"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" s="20">
+      <c r="A149" s="17">
         <v>43991</v>
       </c>
-      <c r="B149" s="24"/>
-      <c r="C149" s="23"/>
+      <c r="B149" s="21"/>
+      <c r="C149" s="20"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="20">
+      <c r="A150" s="17">
         <v>43992</v>
       </c>
-      <c r="B150" s="24"/>
-      <c r="C150" s="23"/>
+      <c r="B150" s="21"/>
+      <c r="C150" s="20"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A151" s="20">
+      <c r="A151" s="17">
         <v>43993</v>
       </c>
-      <c r="B151" s="24"/>
-      <c r="C151" s="23"/>
+      <c r="B151" s="21"/>
+      <c r="C151" s="20"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A152" s="20">
+      <c r="A152" s="17">
         <v>43994</v>
       </c>
-      <c r="B152" s="24"/>
-      <c r="C152" s="23"/>
+      <c r="B152" s="21"/>
+      <c r="C152" s="20"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" s="20">
+      <c r="A153" s="17">
         <v>43995</v>
       </c>
-      <c r="B153" s="24"/>
-      <c r="C153" s="23"/>
+      <c r="B153" s="21"/>
+      <c r="C153" s="20"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" s="20">
+      <c r="A154" s="17">
         <v>43996</v>
       </c>
-      <c r="B154" s="24"/>
-      <c r="C154" s="23"/>
+      <c r="B154" s="21"/>
+      <c r="C154" s="20"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A155" s="20">
+      <c r="A155" s="17">
         <v>43997</v>
       </c>
-      <c r="B155" s="24"/>
-      <c r="C155" s="23"/>
+      <c r="B155" s="21"/>
+      <c r="C155" s="20"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A156" s="21"/>
+      <c r="A156" s="18"/>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A157" s="21"/>
+      <c r="A157" s="18"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A158" s="21"/>
+      <c r="A158" s="18"/>
     </row>
     <row r="159" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C159" s="13">
+      <c r="C159" s="12">
         <f>SUM(C64:C155)</f>
         <v>21</v>
       </c>
-      <c r="F159" s="6">
+      <c r="F159" s="5">
         <f>SUM(F2:F155)</f>
         <v>0</v>
       </c>
-      <c r="I159" s="7">
+      <c r="I159" s="6">
         <f>SUM(I2:I155)</f>
         <v>0</v>
       </c>
-      <c r="L159" s="7">
+      <c r="L159" s="6">
         <f>SUM(L2:L155)</f>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B2:C63"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E2:F63"/>
+    <mergeCell ref="F65:F68"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="B2:C63"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="E69:F70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>